<commit_message>
The Copenhagen Scraper is finialised.
This is also noted in the excel sheet.
The structure of the municipality of Copenhagen, made it so that each item in all of the meetings have their own archive file. This is because each item had it's own webpage.
</commit_message>
<xml_diff>
--- a/Kommuner.xlsx
+++ b/Kommuner.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\musse\OneDrive\UNI\9. semester\GitHub\First_Repository_CROW_FAR\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="79" documentId="11_FCF7A8DB0547560E5E40D026441A350C98F132E0" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{8DEBF043-17B2-4E2A-8462-C363F239BE6E}"/>
+  <xr:revisionPtr revIDLastSave="81" documentId="11_FCF7A8DB0547560E5E40D026441A350C98F132E0" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{82BE9B03-DC11-4678-BA24-53B7CDC0DE82}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="9350" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="291">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="339" uniqueCount="292">
   <si>
     <t>Kommuner</t>
   </si>
@@ -68,9 +68,6 @@
     <t>Massimo</t>
   </si>
   <si>
-    <t>Coding done - download needed</t>
-  </si>
-  <si>
     <t>Aarhus</t>
   </si>
   <si>
@@ -903,6 +900,12 @@
   </si>
   <si>
     <t>Got old code</t>
+  </si>
+  <si>
+    <t>Coding done - download started</t>
+  </si>
+  <si>
+    <t>2007 - 2017</t>
   </si>
 </sst>
 </file>
@@ -1298,7 +1301,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
+      <selection pane="bottomLeft" activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1356,70 +1359,72 @@
         <v>11</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="H2" s="1"/>
+        <v>290</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>291</v>
+      </c>
       <c r="I2" s="1"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" t="s">
         <v>13</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" s="6" t="s">
         <v>14</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>15</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3">
         <v>340421</v>
       </c>
       <c r="F3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="H3" s="1" t="s">
         <v>17</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>18</v>
       </c>
       <c r="I3" s="1"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" t="s">
         <v>19</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" s="6" t="s">
         <v>20</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>21</v>
       </c>
       <c r="D4" s="1"/>
       <c r="E4">
         <v>213558</v>
       </c>
       <c r="F4" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G4" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="H4" s="1" t="s">
         <v>23</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>24</v>
       </c>
       <c r="I4" s="1"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" t="s">
         <v>25</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" s="6" t="s">
         <v>26</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>27</v>
       </c>
       <c r="E5">
         <v>202348</v>
@@ -1430,10 +1435,10 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B6" t="s">
         <v>28</v>
-      </c>
-      <c r="B6" t="s">
-        <v>29</v>
       </c>
       <c r="E6">
         <v>116032</v>
@@ -1444,13 +1449,13 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
+        <v>29</v>
+      </c>
+      <c r="B7" t="s">
         <v>30</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" s="6" t="s">
         <v>31</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>32</v>
       </c>
       <c r="E7">
         <v>114140</v>
@@ -1461,13 +1466,13 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
+        <v>32</v>
+      </c>
+      <c r="B8" t="s">
         <v>33</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" s="6" t="s">
         <v>34</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>35</v>
       </c>
       <c r="D8" s="1"/>
       <c r="E8">
@@ -1480,13 +1485,13 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
+        <v>35</v>
+      </c>
+      <c r="B9" t="s">
         <v>36</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C9" s="6" t="s">
         <v>37</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>38</v>
       </c>
       <c r="E9">
         <v>98265</v>
@@ -1497,16 +1502,16 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
+        <v>38</v>
+      </c>
+      <c r="B10" t="s">
         <v>39</v>
       </c>
-      <c r="B10" t="s">
+      <c r="C10" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="C10" s="6" t="s">
+      <c r="D10" s="4" t="s">
         <v>41</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>42</v>
       </c>
       <c r="E10">
         <v>96883</v>
@@ -1518,16 +1523,16 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
+        <v>42</v>
+      </c>
+      <c r="B11" t="s">
         <v>43</v>
       </c>
-      <c r="B11" t="s">
+      <c r="C11" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="C11" s="6" t="s">
+      <c r="D11" s="6" t="s">
         <v>45</v>
-      </c>
-      <c r="D11" s="6" t="s">
-        <v>46</v>
       </c>
       <c r="E11">
         <v>92515</v>
@@ -1539,13 +1544,13 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
+        <v>46</v>
+      </c>
+      <c r="B12" t="s">
         <v>47</v>
       </c>
-      <c r="B12" t="s">
+      <c r="C12" s="6" t="s">
         <v>48</v>
-      </c>
-      <c r="C12" s="6" t="s">
-        <v>49</v>
       </c>
       <c r="D12" s="1"/>
       <c r="E12">
@@ -1558,13 +1563,13 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
+        <v>49</v>
+      </c>
+      <c r="B13" t="s">
         <v>50</v>
       </c>
-      <c r="B13" t="s">
+      <c r="C13" s="6" t="s">
         <v>51</v>
-      </c>
-      <c r="C13" s="6" t="s">
-        <v>52</v>
       </c>
       <c r="D13" s="1"/>
       <c r="E13">
@@ -1577,13 +1582,13 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
+        <v>52</v>
+      </c>
+      <c r="B14" t="s">
         <v>53</v>
       </c>
-      <c r="B14" t="s">
+      <c r="C14" s="6" t="s">
         <v>54</v>
-      </c>
-      <c r="C14" s="6" t="s">
-        <v>55</v>
       </c>
       <c r="D14" s="1"/>
       <c r="E14">
@@ -1596,13 +1601,13 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
+        <v>55</v>
+      </c>
+      <c r="B15" t="s">
         <v>56</v>
       </c>
-      <c r="B15" t="s">
+      <c r="C15" s="6" t="s">
         <v>57</v>
-      </c>
-      <c r="C15" s="6" t="s">
-        <v>58</v>
       </c>
       <c r="E15">
         <v>87382</v>
@@ -1613,16 +1618,16 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
+        <v>58</v>
+      </c>
+      <c r="B16" t="s">
         <v>59</v>
       </c>
-      <c r="B16" t="s">
+      <c r="C16" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="C16" s="6" t="s">
+      <c r="D16" s="6" t="s">
         <v>61</v>
-      </c>
-      <c r="D16" s="6" t="s">
-        <v>62</v>
       </c>
       <c r="E16">
         <v>82937</v>
@@ -1634,13 +1639,13 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
+        <v>62</v>
+      </c>
+      <c r="B17" t="s">
         <v>63</v>
       </c>
-      <c r="B17" t="s">
+      <c r="C17" s="6" t="s">
         <v>64</v>
-      </c>
-      <c r="C17" s="6" t="s">
-        <v>65</v>
       </c>
       <c r="D17" s="1"/>
       <c r="E17">
@@ -1653,13 +1658,13 @@
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
+        <v>65</v>
+      </c>
+      <c r="B18" t="s">
         <v>66</v>
       </c>
-      <c r="B18" t="s">
+      <c r="C18" s="6" t="s">
         <v>67</v>
-      </c>
-      <c r="C18" s="6" t="s">
-        <v>68</v>
       </c>
       <c r="D18" s="1"/>
       <c r="E18">
@@ -1672,13 +1677,13 @@
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
+        <v>68</v>
+      </c>
+      <c r="B19" t="s">
         <v>69</v>
       </c>
-      <c r="B19" t="s">
+      <c r="C19" s="6" t="s">
         <v>70</v>
-      </c>
-      <c r="C19" s="6" t="s">
-        <v>71</v>
       </c>
       <c r="D19" s="1"/>
       <c r="E19">
@@ -1691,16 +1696,16 @@
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
+        <v>71</v>
+      </c>
+      <c r="B20" t="s">
+        <v>50</v>
+      </c>
+      <c r="C20" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="B20" t="s">
-        <v>51</v>
-      </c>
-      <c r="C20" s="6" t="s">
+      <c r="D20" s="6" t="s">
         <v>73</v>
-      </c>
-      <c r="D20" s="6" t="s">
-        <v>74</v>
       </c>
       <c r="E20">
         <v>70983</v>
@@ -1712,16 +1717,16 @@
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
+        <v>74</v>
+      </c>
+      <c r="B21" t="s">
         <v>75</v>
       </c>
-      <c r="B21" t="s">
+      <c r="C21" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="C21" s="6" t="s">
+      <c r="D21" s="6" t="s">
         <v>77</v>
-      </c>
-      <c r="D21" s="6" t="s">
-        <v>78</v>
       </c>
       <c r="E21">
         <v>69484</v>
@@ -1733,13 +1738,13 @@
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
+        <v>78</v>
+      </c>
+      <c r="B22" t="s">
         <v>79</v>
       </c>
-      <c r="B22" t="s">
+      <c r="C22" s="6" t="s">
         <v>80</v>
-      </c>
-      <c r="C22" s="6" t="s">
-        <v>81</v>
       </c>
       <c r="D22" s="1"/>
       <c r="E22">
@@ -1752,13 +1757,13 @@
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
+        <v>81</v>
+      </c>
+      <c r="B23" t="s">
+        <v>19</v>
+      </c>
+      <c r="C23" s="6" t="s">
         <v>82</v>
-      </c>
-      <c r="B23" t="s">
-        <v>20</v>
-      </c>
-      <c r="C23" s="6" t="s">
-        <v>83</v>
       </c>
       <c r="D23" s="1"/>
       <c r="E23">
@@ -1771,13 +1776,13 @@
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
+        <v>83</v>
+      </c>
+      <c r="B24" t="s">
         <v>84</v>
       </c>
-      <c r="B24" t="s">
+      <c r="C24" s="6" t="s">
         <v>85</v>
-      </c>
-      <c r="C24" s="6" t="s">
-        <v>86</v>
       </c>
       <c r="D24" s="1"/>
       <c r="E24">
@@ -1790,13 +1795,13 @@
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
+        <v>86</v>
+      </c>
+      <c r="B25" t="s">
+        <v>56</v>
+      </c>
+      <c r="C25" s="6" t="s">
         <v>87</v>
-      </c>
-      <c r="B25" t="s">
-        <v>57</v>
-      </c>
-      <c r="C25" s="6" t="s">
-        <v>88</v>
       </c>
       <c r="D25" s="1"/>
       <c r="E25">
@@ -1809,13 +1814,13 @@
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
+        <v>88</v>
+      </c>
+      <c r="B26" t="s">
         <v>89</v>
       </c>
-      <c r="B26" t="s">
+      <c r="C26" s="6" t="s">
         <v>90</v>
-      </c>
-      <c r="C26" s="6" t="s">
-        <v>91</v>
       </c>
       <c r="E26">
         <v>60356</v>
@@ -1826,16 +1831,16 @@
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
+        <v>91</v>
+      </c>
+      <c r="B27" t="s">
         <v>92</v>
       </c>
-      <c r="B27" t="s">
+      <c r="C27" s="6" t="s">
         <v>93</v>
       </c>
-      <c r="C27" s="6" t="s">
+      <c r="D27" s="6" t="s">
         <v>94</v>
-      </c>
-      <c r="D27" s="6" t="s">
-        <v>95</v>
       </c>
       <c r="E27">
         <v>60140</v>
@@ -1847,13 +1852,13 @@
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
+        <v>95</v>
+      </c>
+      <c r="B28" t="s">
         <v>96</v>
       </c>
-      <c r="B28" t="s">
+      <c r="C28" s="6" t="s">
         <v>97</v>
-      </c>
-      <c r="C28" s="6" t="s">
-        <v>98</v>
       </c>
       <c r="D28" s="1"/>
       <c r="E28">
@@ -1866,13 +1871,13 @@
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
+        <v>98</v>
+      </c>
+      <c r="B29" t="s">
         <v>99</v>
       </c>
-      <c r="B29" t="s">
+      <c r="C29" s="6" t="s">
         <v>100</v>
-      </c>
-      <c r="C29" s="6" t="s">
-        <v>101</v>
       </c>
       <c r="E29">
         <v>58698</v>
@@ -1883,13 +1888,13 @@
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
+        <v>101</v>
+      </c>
+      <c r="B30" t="s">
         <v>102</v>
       </c>
-      <c r="B30" t="s">
+      <c r="C30" s="6" t="s">
         <v>103</v>
-      </c>
-      <c r="C30" s="6" t="s">
-        <v>104</v>
       </c>
       <c r="D30" s="1"/>
       <c r="E30">
@@ -1902,13 +1907,13 @@
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
+        <v>104</v>
+      </c>
+      <c r="B31" t="s">
         <v>105</v>
       </c>
-      <c r="B31" t="s">
+      <c r="C31" s="6" t="s">
         <v>106</v>
-      </c>
-      <c r="C31" s="6" t="s">
-        <v>107</v>
       </c>
       <c r="D31" s="1"/>
       <c r="E31">
@@ -1921,13 +1926,13 @@
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
+        <v>107</v>
+      </c>
+      <c r="B32" t="s">
+        <v>19</v>
+      </c>
+      <c r="C32" s="6" t="s">
         <v>108</v>
-      </c>
-      <c r="B32" t="s">
-        <v>20</v>
-      </c>
-      <c r="C32" s="6" t="s">
-        <v>109</v>
       </c>
       <c r="D32" s="1"/>
       <c r="E32">
@@ -1940,10 +1945,10 @@
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
+        <v>109</v>
+      </c>
+      <c r="B33" s="3" t="s">
         <v>110</v>
-      </c>
-      <c r="B33" s="3" t="s">
-        <v>111</v>
       </c>
       <c r="E33">
         <v>55963</v>
@@ -1954,13 +1959,13 @@
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
+        <v>111</v>
+      </c>
+      <c r="B34" t="s">
         <v>112</v>
       </c>
-      <c r="B34" t="s">
+      <c r="C34" s="6" t="s">
         <v>113</v>
-      </c>
-      <c r="C34" s="6" t="s">
-        <v>114</v>
       </c>
       <c r="D34" s="1"/>
       <c r="E34">
@@ -1973,16 +1978,16 @@
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
+        <v>114</v>
+      </c>
+      <c r="B35" t="s">
+        <v>56</v>
+      </c>
+      <c r="C35" s="6" t="s">
         <v>115</v>
       </c>
-      <c r="B35" t="s">
-        <v>57</v>
-      </c>
-      <c r="C35" s="6" t="s">
+      <c r="D35" s="4" t="s">
         <v>116</v>
-      </c>
-      <c r="D35" s="4" t="s">
-        <v>117</v>
       </c>
       <c r="E35">
         <v>53282</v>
@@ -1994,13 +1999,13 @@
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
+        <v>117</v>
+      </c>
+      <c r="B36" t="s">
+        <v>75</v>
+      </c>
+      <c r="C36" s="6" t="s">
         <v>118</v>
-      </c>
-      <c r="B36" t="s">
-        <v>76</v>
-      </c>
-      <c r="C36" s="6" t="s">
-        <v>119</v>
       </c>
       <c r="D36" s="1"/>
       <c r="E36">
@@ -2013,13 +2018,13 @@
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
+        <v>119</v>
+      </c>
+      <c r="B37" t="s">
         <v>120</v>
       </c>
-      <c r="B37" t="s">
+      <c r="C37" s="6" t="s">
         <v>121</v>
-      </c>
-      <c r="C37" s="6" t="s">
-        <v>122</v>
       </c>
       <c r="D37" s="1"/>
       <c r="E37">
@@ -2032,16 +2037,16 @@
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
+        <v>122</v>
+      </c>
+      <c r="B38" t="s">
         <v>123</v>
       </c>
-      <c r="B38" t="s">
+      <c r="C38" s="6" t="s">
         <v>124</v>
       </c>
-      <c r="C38" s="6" t="s">
+      <c r="D38" s="6" t="s">
         <v>125</v>
-      </c>
-      <c r="D38" s="6" t="s">
-        <v>126</v>
       </c>
       <c r="E38">
         <v>50650</v>
@@ -2053,13 +2058,13 @@
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
+        <v>126</v>
+      </c>
+      <c r="B39" t="s">
+        <v>19</v>
+      </c>
+      <c r="C39" s="6" t="s">
         <v>127</v>
-      </c>
-      <c r="B39" t="s">
-        <v>20</v>
-      </c>
-      <c r="C39" s="6" t="s">
-        <v>128</v>
       </c>
       <c r="D39" s="1"/>
       <c r="E39">
@@ -2072,16 +2077,16 @@
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
+        <v>128</v>
+      </c>
+      <c r="B40" t="s">
         <v>129</v>
       </c>
-      <c r="B40" t="s">
+      <c r="C40" s="6" t="s">
         <v>130</v>
       </c>
-      <c r="C40" s="6" t="s">
+      <c r="D40" s="4" t="s">
         <v>131</v>
-      </c>
-      <c r="D40" s="4" t="s">
-        <v>132</v>
       </c>
       <c r="E40">
         <v>50301</v>
@@ -2093,13 +2098,13 @@
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
+        <v>132</v>
+      </c>
+      <c r="B41" t="s">
+        <v>63</v>
+      </c>
+      <c r="C41" s="6" t="s">
         <v>133</v>
-      </c>
-      <c r="B41" t="s">
-        <v>64</v>
-      </c>
-      <c r="C41" s="6" t="s">
-        <v>134</v>
       </c>
       <c r="E41">
         <v>49974</v>
@@ -2110,13 +2115,13 @@
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
+        <v>134</v>
+      </c>
+      <c r="B42" t="s">
+        <v>63</v>
+      </c>
+      <c r="C42" s="6" t="s">
         <v>135</v>
-      </c>
-      <c r="B42" t="s">
-        <v>64</v>
-      </c>
-      <c r="C42" s="6" t="s">
-        <v>136</v>
       </c>
       <c r="D42" s="1"/>
       <c r="E42">
@@ -2129,13 +2134,13 @@
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
+        <v>136</v>
+      </c>
+      <c r="B43" t="s">
+        <v>66</v>
+      </c>
+      <c r="C43" s="6" t="s">
         <v>137</v>
-      </c>
-      <c r="B43" t="s">
-        <v>67</v>
-      </c>
-      <c r="C43" s="6" t="s">
-        <v>138</v>
       </c>
       <c r="D43" s="1"/>
       <c r="E43">
@@ -2148,13 +2153,13 @@
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
+        <v>138</v>
+      </c>
+      <c r="B44" t="s">
+        <v>63</v>
+      </c>
+      <c r="C44" s="6" t="s">
         <v>139</v>
-      </c>
-      <c r="B44" t="s">
-        <v>64</v>
-      </c>
-      <c r="C44" s="6" t="s">
-        <v>140</v>
       </c>
       <c r="E44">
         <v>48271</v>
@@ -2165,13 +2170,13 @@
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
+        <v>140</v>
+      </c>
+      <c r="B45" t="s">
         <v>141</v>
       </c>
-      <c r="B45" t="s">
+      <c r="C45" s="6" t="s">
         <v>142</v>
-      </c>
-      <c r="C45" s="6" t="s">
-        <v>143</v>
       </c>
       <c r="D45" s="1"/>
       <c r="E45">
@@ -2184,13 +2189,13 @@
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
+        <v>143</v>
+      </c>
+      <c r="B46" t="s">
+        <v>63</v>
+      </c>
+      <c r="C46" s="6" t="s">
         <v>144</v>
-      </c>
-      <c r="B46" t="s">
-        <v>64</v>
-      </c>
-      <c r="C46" s="6" t="s">
-        <v>145</v>
       </c>
       <c r="D46" s="1"/>
       <c r="E46">
@@ -2200,23 +2205,23 @@
         <v>11</v>
       </c>
       <c r="G46" s="1" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="H46" s="1"/>
       <c r="I46" s="1"/>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
+        <v>145</v>
+      </c>
+      <c r="B47" t="s">
         <v>146</v>
       </c>
-      <c r="B47" t="s">
+      <c r="C47" s="6" t="s">
         <v>147</v>
       </c>
-      <c r="C47" s="6" t="s">
+      <c r="D47" s="6" t="s">
         <v>148</v>
-      </c>
-      <c r="D47" s="6" t="s">
-        <v>149</v>
       </c>
       <c r="E47">
         <v>46087</v>
@@ -2227,13 +2232,13 @@
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
+        <v>149</v>
+      </c>
+      <c r="B48" t="s">
         <v>150</v>
       </c>
-      <c r="B48" t="s">
+      <c r="C48" s="6" t="s">
         <v>151</v>
-      </c>
-      <c r="C48" s="6" t="s">
-        <v>152</v>
       </c>
       <c r="E48">
         <v>45189</v>
@@ -2244,16 +2249,16 @@
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
+        <v>152</v>
+      </c>
+      <c r="B49" t="s">
+        <v>56</v>
+      </c>
+      <c r="C49" s="6" t="s">
         <v>153</v>
       </c>
-      <c r="B49" t="s">
-        <v>57</v>
-      </c>
-      <c r="C49" s="6" t="s">
+      <c r="D49" s="4" t="s">
         <v>154</v>
-      </c>
-      <c r="D49" s="4" t="s">
-        <v>155</v>
       </c>
       <c r="E49">
         <v>43716</v>
@@ -2265,13 +2270,13 @@
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
+        <v>155</v>
+      </c>
+      <c r="B50" s="7" t="s">
         <v>156</v>
       </c>
-      <c r="B50" s="7" t="s">
+      <c r="C50" s="6" t="s">
         <v>157</v>
-      </c>
-      <c r="C50" s="6" t="s">
-        <v>158</v>
       </c>
       <c r="D50" s="1"/>
       <c r="E50">
@@ -2284,13 +2289,13 @@
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
+        <v>158</v>
+      </c>
+      <c r="B51" t="s">
+        <v>56</v>
+      </c>
+      <c r="C51" s="6" t="s">
         <v>159</v>
-      </c>
-      <c r="B51" t="s">
-        <v>57</v>
-      </c>
-      <c r="C51" s="6" t="s">
-        <v>160</v>
       </c>
       <c r="D51" s="1"/>
       <c r="E51">
@@ -2303,13 +2308,13 @@
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
+        <v>160</v>
+      </c>
+      <c r="B52" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="C52" s="6" t="s">
         <v>161</v>
-      </c>
-      <c r="B52" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="C52" s="6" t="s">
-        <v>162</v>
       </c>
       <c r="D52" s="1"/>
       <c r="E52">
@@ -2322,13 +2327,13 @@
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
+        <v>162</v>
+      </c>
+      <c r="B53" t="s">
+        <v>66</v>
+      </c>
+      <c r="C53" t="s">
         <v>163</v>
-      </c>
-      <c r="B53" t="s">
-        <v>67</v>
-      </c>
-      <c r="C53" t="s">
-        <v>164</v>
       </c>
       <c r="D53" s="1"/>
       <c r="E53">
@@ -2338,20 +2343,20 @@
         <v>11</v>
       </c>
       <c r="G53" s="9" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="H53" s="1"/>
       <c r="I53" s="1"/>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
+        <v>164</v>
+      </c>
+      <c r="B54" t="s">
+        <v>19</v>
+      </c>
+      <c r="C54" s="6" t="s">
         <v>165</v>
-      </c>
-      <c r="B54" t="s">
-        <v>20</v>
-      </c>
-      <c r="C54" s="6" t="s">
-        <v>166</v>
       </c>
       <c r="D54" s="1"/>
       <c r="E54">
@@ -2364,13 +2369,13 @@
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
+        <v>166</v>
+      </c>
+      <c r="B55" t="s">
         <v>167</v>
       </c>
-      <c r="B55" t="s">
+      <c r="C55" s="6" t="s">
         <v>168</v>
-      </c>
-      <c r="C55" s="6" t="s">
-        <v>169</v>
       </c>
       <c r="D55" s="1"/>
       <c r="E55">
@@ -2383,13 +2388,13 @@
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
+        <v>169</v>
+      </c>
+      <c r="B56" t="s">
         <v>170</v>
       </c>
-      <c r="B56" t="s">
+      <c r="C56" s="6" t="s">
         <v>171</v>
-      </c>
-      <c r="C56" s="6" t="s">
-        <v>172</v>
       </c>
       <c r="D56" s="1"/>
       <c r="E56">
@@ -2402,16 +2407,16 @@
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
+        <v>172</v>
+      </c>
+      <c r="B57" t="s">
+        <v>33</v>
+      </c>
+      <c r="C57" s="6" t="s">
         <v>173</v>
       </c>
-      <c r="B57" t="s">
-        <v>34</v>
-      </c>
-      <c r="C57" s="6" t="s">
+      <c r="D57" s="6" t="s">
         <v>174</v>
-      </c>
-      <c r="D57" s="6" t="s">
-        <v>175</v>
       </c>
       <c r="E57">
         <v>41217</v>
@@ -2422,13 +2427,13 @@
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
+        <v>175</v>
+      </c>
+      <c r="B58" t="s">
         <v>176</v>
       </c>
-      <c r="B58" t="s">
+      <c r="C58" s="6" t="s">
         <v>177</v>
-      </c>
-      <c r="C58" s="6" t="s">
-        <v>178</v>
       </c>
       <c r="D58" s="1"/>
       <c r="E58">
@@ -2441,16 +2446,16 @@
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
+        <v>178</v>
+      </c>
+      <c r="B59" t="s">
         <v>179</v>
       </c>
-      <c r="B59" t="s">
+      <c r="C59" s="6" t="s">
         <v>180</v>
       </c>
-      <c r="C59" s="6" t="s">
+      <c r="D59" s="6" t="s">
         <v>181</v>
-      </c>
-      <c r="D59" s="6" t="s">
-        <v>182</v>
       </c>
       <c r="E59">
         <v>40911</v>
@@ -2462,13 +2467,13 @@
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
+        <v>182</v>
+      </c>
+      <c r="B60" t="s">
         <v>183</v>
       </c>
-      <c r="B60" t="s">
+      <c r="C60" s="6" t="s">
         <v>184</v>
-      </c>
-      <c r="C60" s="6" t="s">
-        <v>185</v>
       </c>
       <c r="D60" s="1"/>
       <c r="E60">
@@ -2481,13 +2486,13 @@
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
+        <v>185</v>
+      </c>
+      <c r="B61" t="s">
         <v>186</v>
       </c>
-      <c r="B61" t="s">
+      <c r="C61" s="6" t="s">
         <v>187</v>
-      </c>
-      <c r="C61" s="6" t="s">
-        <v>188</v>
       </c>
       <c r="D61" s="1"/>
       <c r="E61">
@@ -2500,13 +2505,13 @@
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
+        <v>188</v>
+      </c>
+      <c r="B62" t="s">
         <v>189</v>
       </c>
-      <c r="B62" t="s">
+      <c r="C62" s="6" t="s">
         <v>190</v>
-      </c>
-      <c r="C62" s="6" t="s">
-        <v>191</v>
       </c>
       <c r="D62" s="1"/>
       <c r="E62">
@@ -2519,16 +2524,16 @@
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
+        <v>191</v>
+      </c>
+      <c r="B63" t="s">
         <v>192</v>
       </c>
-      <c r="B63" t="s">
+      <c r="C63" s="6" t="s">
         <v>193</v>
       </c>
-      <c r="C63" s="6" t="s">
+      <c r="D63" s="6" t="s">
         <v>194</v>
-      </c>
-      <c r="D63" s="6" t="s">
-        <v>195</v>
       </c>
       <c r="E63">
         <v>38638</v>
@@ -2540,13 +2545,13 @@
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
+        <v>195</v>
+      </c>
+      <c r="B64" t="s">
         <v>196</v>
       </c>
-      <c r="B64" t="s">
+      <c r="C64" s="6" t="s">
         <v>197</v>
-      </c>
-      <c r="C64" s="6" t="s">
-        <v>198</v>
       </c>
       <c r="D64" s="1"/>
       <c r="E64">
@@ -2559,16 +2564,16 @@
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
+        <v>198</v>
+      </c>
+      <c r="B65" t="s">
         <v>199</v>
       </c>
-      <c r="B65" t="s">
+      <c r="C65" s="6" t="s">
         <v>200</v>
       </c>
-      <c r="C65" s="6" t="s">
+      <c r="D65" s="6" t="s">
         <v>201</v>
-      </c>
-      <c r="D65" s="6" t="s">
-        <v>202</v>
       </c>
       <c r="E65">
         <v>38197</v>
@@ -2579,13 +2584,13 @@
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
+        <v>202</v>
+      </c>
+      <c r="B66" s="5" t="s">
         <v>203</v>
       </c>
-      <c r="B66" s="5" t="s">
+      <c r="C66" s="6" t="s">
         <v>204</v>
-      </c>
-      <c r="C66" s="6" t="s">
-        <v>205</v>
       </c>
       <c r="D66" s="1"/>
       <c r="E66">
@@ -2598,13 +2603,13 @@
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
+        <v>205</v>
+      </c>
+      <c r="B67" t="s">
         <v>206</v>
       </c>
-      <c r="B67" t="s">
+      <c r="C67" s="6" t="s">
         <v>207</v>
-      </c>
-      <c r="C67" s="6" t="s">
-        <v>208</v>
       </c>
       <c r="D67" s="1"/>
       <c r="E67">
@@ -2617,13 +2622,13 @@
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
+        <v>208</v>
+      </c>
+      <c r="B68" t="s">
+        <v>56</v>
+      </c>
+      <c r="C68" s="6" t="s">
         <v>209</v>
-      </c>
-      <c r="B68" t="s">
-        <v>57</v>
-      </c>
-      <c r="C68" s="6" t="s">
-        <v>210</v>
       </c>
       <c r="D68" s="1"/>
       <c r="E68">
@@ -2636,13 +2641,13 @@
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
+        <v>210</v>
+      </c>
+      <c r="B69" t="s">
+        <v>120</v>
+      </c>
+      <c r="C69" s="6" t="s">
         <v>211</v>
-      </c>
-      <c r="B69" t="s">
-        <v>121</v>
-      </c>
-      <c r="C69" s="6" t="s">
-        <v>212</v>
       </c>
       <c r="E69">
         <v>36139</v>
@@ -2653,13 +2658,13 @@
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
+        <v>212</v>
+      </c>
+      <c r="B70" t="s">
+        <v>63</v>
+      </c>
+      <c r="C70" s="6" t="s">
         <v>213</v>
-      </c>
-      <c r="B70" t="s">
-        <v>64</v>
-      </c>
-      <c r="C70" s="6" t="s">
-        <v>214</v>
       </c>
       <c r="D70" s="1"/>
       <c r="E70">
@@ -2672,13 +2677,13 @@
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
+        <v>214</v>
+      </c>
+      <c r="B71" t="s">
+        <v>30</v>
+      </c>
+      <c r="C71" s="6" t="s">
         <v>215</v>
-      </c>
-      <c r="B71" t="s">
-        <v>31</v>
-      </c>
-      <c r="C71" s="6" t="s">
-        <v>216</v>
       </c>
       <c r="D71" s="1"/>
       <c r="E71">
@@ -2691,13 +2696,13 @@
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
+        <v>216</v>
+      </c>
+      <c r="B72" t="s">
+        <v>63</v>
+      </c>
+      <c r="C72" t="s">
         <v>217</v>
-      </c>
-      <c r="B72" t="s">
-        <v>64</v>
-      </c>
-      <c r="C72" t="s">
-        <v>218</v>
       </c>
       <c r="D72" s="1"/>
       <c r="E72">
@@ -2707,20 +2712,20 @@
         <v>11</v>
       </c>
       <c r="G72" s="1" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="H72" s="1"/>
       <c r="I72" s="1"/>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
+        <v>218</v>
+      </c>
+      <c r="B73" t="s">
         <v>219</v>
       </c>
-      <c r="B73" t="s">
+      <c r="C73" s="6" t="s">
         <v>220</v>
-      </c>
-      <c r="C73" s="6" t="s">
-        <v>221</v>
       </c>
       <c r="D73" s="1"/>
       <c r="E73">
@@ -2733,13 +2738,13 @@
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
+        <v>221</v>
+      </c>
+      <c r="B74" t="s">
+        <v>56</v>
+      </c>
+      <c r="C74" s="6" t="s">
         <v>222</v>
-      </c>
-      <c r="B74" t="s">
-        <v>57</v>
-      </c>
-      <c r="C74" s="6" t="s">
-        <v>223</v>
       </c>
       <c r="D74" s="1"/>
       <c r="E74">
@@ -2752,16 +2757,16 @@
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
+        <v>223</v>
+      </c>
+      <c r="B75" t="s">
+        <v>30</v>
+      </c>
+      <c r="C75" s="6" t="s">
         <v>224</v>
       </c>
-      <c r="B75" t="s">
-        <v>31</v>
-      </c>
-      <c r="C75" s="6" t="s">
+      <c r="D75" s="6" t="s">
         <v>225</v>
-      </c>
-      <c r="D75" s="6" t="s">
-        <v>226</v>
       </c>
       <c r="E75">
         <v>29827</v>
@@ -2772,13 +2777,13 @@
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
+        <v>226</v>
+      </c>
+      <c r="B76" t="s">
+        <v>63</v>
+      </c>
+      <c r="C76" t="s">
         <v>227</v>
-      </c>
-      <c r="B76" t="s">
-        <v>64</v>
-      </c>
-      <c r="C76" t="s">
-        <v>228</v>
       </c>
       <c r="D76" s="1"/>
       <c r="E76">
@@ -2788,23 +2793,23 @@
         <v>11</v>
       </c>
       <c r="G76" s="1" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="H76" s="9"/>
       <c r="I76" s="1"/>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
+        <v>228</v>
+      </c>
+      <c r="B77" t="s">
         <v>229</v>
       </c>
-      <c r="B77" t="s">
+      <c r="C77" s="6" t="s">
         <v>230</v>
       </c>
-      <c r="C77" s="6" t="s">
+      <c r="D77" s="6" t="s">
         <v>231</v>
-      </c>
-      <c r="D77" s="6" t="s">
-        <v>232</v>
       </c>
       <c r="E77">
         <v>29516</v>
@@ -2816,10 +2821,10 @@
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
+        <v>232</v>
+      </c>
+      <c r="B78" t="s">
         <v>233</v>
-      </c>
-      <c r="B78" t="s">
-        <v>234</v>
       </c>
       <c r="D78" s="1"/>
       <c r="E78">
@@ -2832,16 +2837,16 @@
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
+        <v>234</v>
+      </c>
+      <c r="B79" t="s">
+        <v>33</v>
+      </c>
+      <c r="C79" s="6" t="s">
         <v>235</v>
       </c>
-      <c r="B79" t="s">
-        <v>34</v>
-      </c>
-      <c r="C79" s="6" t="s">
+      <c r="D79" s="6" t="s">
         <v>236</v>
-      </c>
-      <c r="D79" s="6" t="s">
-        <v>237</v>
       </c>
       <c r="E79">
         <v>27743</v>
@@ -2853,13 +2858,13 @@
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
+        <v>237</v>
+      </c>
+      <c r="B80" t="s">
         <v>238</v>
       </c>
-      <c r="B80" t="s">
+      <c r="C80" s="6" t="s">
         <v>239</v>
-      </c>
-      <c r="C80" s="6" t="s">
-        <v>240</v>
       </c>
       <c r="D80" s="1"/>
       <c r="E80">
@@ -2872,13 +2877,13 @@
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
+        <v>240</v>
+      </c>
+      <c r="B81" t="s">
+        <v>19</v>
+      </c>
+      <c r="C81" s="6" t="s">
         <v>241</v>
-      </c>
-      <c r="B81" t="s">
-        <v>20</v>
-      </c>
-      <c r="C81" s="6" t="s">
-        <v>242</v>
       </c>
       <c r="D81" s="1"/>
       <c r="E81">
@@ -2891,13 +2896,13 @@
     </row>
     <row r="82" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
+        <v>242</v>
+      </c>
+      <c r="B82" s="3" t="s">
         <v>243</v>
       </c>
-      <c r="B82" s="3" t="s">
+      <c r="C82" s="6" t="s">
         <v>244</v>
-      </c>
-      <c r="C82" s="6" t="s">
-        <v>245</v>
       </c>
       <c r="D82" s="1"/>
       <c r="E82">
@@ -2910,13 +2915,13 @@
     </row>
     <row r="83" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
+        <v>245</v>
+      </c>
+      <c r="B83" t="s">
         <v>246</v>
       </c>
-      <c r="B83" t="s">
+      <c r="C83" s="6" t="s">
         <v>247</v>
-      </c>
-      <c r="C83" s="6" t="s">
-        <v>248</v>
       </c>
       <c r="E83">
         <v>25028</v>
@@ -2927,13 +2932,13 @@
     </row>
     <row r="84" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
+        <v>248</v>
+      </c>
+      <c r="B84" t="s">
         <v>249</v>
       </c>
-      <c r="B84" t="s">
+      <c r="C84" s="6" t="s">
         <v>250</v>
-      </c>
-      <c r="C84" s="6" t="s">
-        <v>251</v>
       </c>
       <c r="D84" s="1"/>
       <c r="E84">
@@ -2946,16 +2951,16 @@
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
+        <v>251</v>
+      </c>
+      <c r="B85" t="s">
         <v>252</v>
       </c>
-      <c r="B85" t="s">
+      <c r="C85" s="6" t="s">
         <v>253</v>
       </c>
-      <c r="C85" s="6" t="s">
+      <c r="D85" s="6" t="s">
         <v>254</v>
-      </c>
-      <c r="D85" s="6" t="s">
-        <v>255</v>
       </c>
       <c r="E85">
         <v>22988</v>
@@ -2966,13 +2971,13 @@
     </row>
     <row r="86" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
+        <v>255</v>
+      </c>
+      <c r="B86" t="s">
         <v>256</v>
       </c>
-      <c r="B86" t="s">
+      <c r="C86" s="6" t="s">
         <v>257</v>
-      </c>
-      <c r="C86" s="6" t="s">
-        <v>258</v>
       </c>
       <c r="D86" s="1"/>
       <c r="E86">
@@ -2985,13 +2990,13 @@
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
+        <v>258</v>
+      </c>
+      <c r="B87" t="s">
+        <v>75</v>
+      </c>
+      <c r="C87" s="6" t="s">
         <v>259</v>
-      </c>
-      <c r="B87" t="s">
-        <v>76</v>
-      </c>
-      <c r="C87" s="6" t="s">
-        <v>260</v>
       </c>
       <c r="D87" s="1"/>
       <c r="E87">
@@ -3004,13 +3009,13 @@
     </row>
     <row r="88" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
+        <v>260</v>
+      </c>
+      <c r="B88" t="s">
         <v>261</v>
       </c>
-      <c r="B88" t="s">
+      <c r="C88" s="6" t="s">
         <v>262</v>
-      </c>
-      <c r="C88" s="6" t="s">
-        <v>263</v>
       </c>
       <c r="D88" s="1"/>
       <c r="E88">
@@ -3023,13 +3028,13 @@
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
+        <v>263</v>
+      </c>
+      <c r="B89" t="s">
+        <v>56</v>
+      </c>
+      <c r="C89" s="6" t="s">
         <v>264</v>
-      </c>
-      <c r="B89" t="s">
-        <v>57</v>
-      </c>
-      <c r="C89" s="6" t="s">
-        <v>265</v>
       </c>
       <c r="D89" s="1"/>
       <c r="E89">
@@ -3042,13 +3047,13 @@
     </row>
     <row r="90" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
+        <v>265</v>
+      </c>
+      <c r="B90" t="s">
         <v>266</v>
       </c>
-      <c r="B90" t="s">
+      <c r="C90" s="6" t="s">
         <v>267</v>
-      </c>
-      <c r="C90" s="6" t="s">
-        <v>268</v>
       </c>
       <c r="D90" s="1"/>
       <c r="E90">
@@ -3061,13 +3066,13 @@
     </row>
     <row r="91" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
+        <v>268</v>
+      </c>
+      <c r="B91" t="s">
+        <v>63</v>
+      </c>
+      <c r="C91" s="6" t="s">
         <v>269</v>
-      </c>
-      <c r="B91" t="s">
-        <v>64</v>
-      </c>
-      <c r="C91" s="6" t="s">
-        <v>270</v>
       </c>
       <c r="E91">
         <v>20514</v>
@@ -3078,13 +3083,13 @@
     </row>
     <row r="92" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
+        <v>270</v>
+      </c>
+      <c r="B92" t="s">
         <v>271</v>
       </c>
-      <c r="B92" t="s">
+      <c r="C92" s="6" t="s">
         <v>272</v>
-      </c>
-      <c r="C92" s="6" t="s">
-        <v>273</v>
       </c>
       <c r="E92">
         <v>20133</v>
@@ -3095,13 +3100,13 @@
     </row>
     <row r="93" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
+        <v>273</v>
+      </c>
+      <c r="B93" t="s">
         <v>274</v>
       </c>
-      <c r="B93" t="s">
+      <c r="C93" s="6" t="s">
         <v>275</v>
-      </c>
-      <c r="C93" s="6" t="s">
-        <v>276</v>
       </c>
       <c r="D93" s="1"/>
       <c r="E93">
@@ -3114,13 +3119,13 @@
     </row>
     <row r="94" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
+        <v>276</v>
+      </c>
+      <c r="B94" t="s">
+        <v>96</v>
+      </c>
+      <c r="C94" s="6" t="s">
         <v>277</v>
-      </c>
-      <c r="B94" t="s">
-        <v>97</v>
-      </c>
-      <c r="C94" s="6" t="s">
-        <v>278</v>
       </c>
       <c r="E94">
         <v>14272</v>
@@ -3131,13 +3136,13 @@
     </row>
     <row r="95" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
+        <v>278</v>
+      </c>
+      <c r="B95" t="s">
+        <v>56</v>
+      </c>
+      <c r="C95" s="6" t="s">
         <v>279</v>
-      </c>
-      <c r="B95" t="s">
-        <v>57</v>
-      </c>
-      <c r="C95" s="6" t="s">
-        <v>280</v>
       </c>
       <c r="D95" s="1"/>
       <c r="E95">
@@ -3150,13 +3155,13 @@
     </row>
     <row r="96" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
+        <v>280</v>
+      </c>
+      <c r="B96" t="s">
+        <v>206</v>
+      </c>
+      <c r="C96" s="6" t="s">
         <v>281</v>
-      </c>
-      <c r="B96" t="s">
-        <v>207</v>
-      </c>
-      <c r="C96" s="6" t="s">
-        <v>282</v>
       </c>
       <c r="E96">
         <v>6178</v>
@@ -3167,13 +3172,13 @@
     </row>
     <row r="97" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
+        <v>282</v>
+      </c>
+      <c r="B97" t="s">
+        <v>63</v>
+      </c>
+      <c r="C97" s="6" t="s">
         <v>283</v>
-      </c>
-      <c r="B97" t="s">
-        <v>64</v>
-      </c>
-      <c r="C97" s="6" t="s">
-        <v>284</v>
       </c>
       <c r="D97" s="1"/>
       <c r="E97">
@@ -3183,20 +3188,20 @@
         <v>11</v>
       </c>
       <c r="G97" s="1" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="H97" s="8"/>
       <c r="I97" s="1"/>
     </row>
     <row r="98" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
+        <v>284</v>
+      </c>
+      <c r="B98" t="s">
+        <v>63</v>
+      </c>
+      <c r="C98" s="6" t="s">
         <v>285</v>
-      </c>
-      <c r="B98" t="s">
-        <v>64</v>
-      </c>
-      <c r="C98" s="6" t="s">
-        <v>286</v>
       </c>
       <c r="E98">
         <v>3401</v>
@@ -3205,18 +3210,18 @@
         <v>11</v>
       </c>
       <c r="G98" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="99" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
+        <v>286</v>
+      </c>
+      <c r="B99" t="s">
         <v>287</v>
       </c>
-      <c r="B99" t="s">
+      <c r="C99" s="6" t="s">
         <v>288</v>
-      </c>
-      <c r="C99" s="6" t="s">
-        <v>289</v>
       </c>
       <c r="E99">
         <v>1807</v>

</xml_diff>

<commit_message>
Scraper for Frederiksberg - done
</commit_message>
<xml_diff>
--- a/Kommuner.xlsx
+++ b/Kommuner.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\musse\OneDrive\UNI\9. semester\GitHub\First_Repository_CROW_FAR\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="83" documentId="11_FCF7A8DB0547560E5E40D026441A350C98F132E0" xr6:coauthVersionLast="41" xr6:coauthVersionMax="43" xr10:uidLastSave="{726AEF9F-F90B-4883-96BB-79974E24FF77}"/>
+  <xr:revisionPtr revIDLastSave="86" documentId="11_FCF7A8DB0547560E5E40D026441A350C98F132E0" xr6:coauthVersionLast="41" xr6:coauthVersionMax="43" xr10:uidLastSave="{9B19172D-676C-4ADA-B769-258C691C5291}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="341" uniqueCount="293">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="292">
   <si>
     <t>Kommuner</t>
   </si>
@@ -902,13 +902,10 @@
     <t>Got old code</t>
   </si>
   <si>
-    <t>Coding done - download started</t>
-  </si>
-  <si>
     <t>2007 - 2017</t>
   </si>
   <si>
-    <t>Started</t>
+    <t>2012 - 2017</t>
   </si>
 </sst>
 </file>
@@ -1304,7 +1301,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
+      <selection pane="bottomLeft" activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1362,10 +1359,10 @@
         <v>11</v>
       </c>
       <c r="G2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" s="1" t="s">
         <v>290</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>291</v>
       </c>
       <c r="I2" s="1"/>
     </row>
@@ -1485,9 +1482,11 @@
         <v>11</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>292</v>
-      </c>
-      <c r="H8" s="1"/>
+        <v>16</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>291</v>
+      </c>
       <c r="I8" s="1"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Made scraper for Gentofte
</commit_message>
<xml_diff>
--- a/Kommuner.xlsx
+++ b/Kommuner.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\musse\OneDrive\UNI\9. semester\GitHub\First_Repository_CROW_FAR\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="26" documentId="11_FDF7A8DB94275223C5388096340570E2CE8365A4" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{10606744-B810-434E-8FF2-3AE2363A96FB}"/>
+  <xr:revisionPtr revIDLastSave="36" documentId="11_FDF7A8DB94275223C5388096340570E2CE8365A4" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{FCB80603-ABC8-4C7F-B82B-2D2B4CD0AAD0}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="298">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="363" uniqueCount="299">
   <si>
     <t>Kommuner</t>
   </si>
@@ -228,18 +228,12 @@
     <t>Sønderborg</t>
   </si>
   <si>
-    <t>PDF - Form</t>
-  </si>
-  <si>
     <t>https://sonderborgkommune.dk/dagsordener</t>
   </si>
   <si>
     <t>Holbæk</t>
   </si>
   <si>
-    <t>https://holbaek.dk/politik/udvalg/</t>
-  </si>
-  <si>
     <t>https://holbaek.dk/politik/referater-2014-2017/</t>
   </si>
   <si>
@@ -919,6 +913,15 @@
   </si>
   <si>
     <t>Underway</t>
+  </si>
+  <si>
+    <t>Files downloaded, not parsed though as items were not readily availeble</t>
+  </si>
+  <si>
+    <t>NOTHING BEFORE 2017 - PDF - Form</t>
+  </si>
+  <si>
+    <t>2018 - 2019</t>
   </si>
 </sst>
 </file>
@@ -1313,14 +1316,14 @@
   <dimension ref="A1:I99"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G23" sqref="G23"/>
+      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="25.26953125" customWidth="1"/>
-    <col min="2" max="2" width="17.453125" customWidth="1"/>
+    <col min="2" max="2" width="24.54296875" customWidth="1"/>
     <col min="3" max="3" width="32.453125" customWidth="1"/>
     <col min="5" max="5" width="12.54296875" customWidth="1"/>
     <col min="6" max="6" width="15.26953125" customWidth="1"/>
@@ -1375,7 +1378,7 @@
         <v>16</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="I2" s="1"/>
     </row>
@@ -1498,7 +1501,7 @@
         <v>16</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="I8" s="1"/>
     </row>
@@ -1561,7 +1564,7 @@
         <v>16</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="I11" s="1"/>
     </row>
@@ -1586,7 +1589,7 @@
         <v>16</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="I12" s="1"/>
     </row>
@@ -1595,7 +1598,7 @@
         <v>49</v>
       </c>
       <c r="B13" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="C13" s="6" t="s">
         <v>51</v>
@@ -1614,7 +1617,7 @@
         <v>52</v>
       </c>
       <c r="B14" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="C14" s="6" t="s">
         <v>53</v>
@@ -1645,10 +1648,10 @@
         <v>11</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="I15" s="1"/>
     </row>
@@ -1657,7 +1660,7 @@
         <v>57</v>
       </c>
       <c r="B16" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="C16" s="6" t="s">
         <v>58</v>
@@ -1672,10 +1675,10 @@
         <v>11</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="I16" s="1"/>
     </row>
@@ -1697,10 +1700,10 @@
         <v>11</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="I17" s="1"/>
     </row>
@@ -1722,10 +1725,10 @@
         <v>11</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="I18" s="1"/>
     </row>
@@ -1734,10 +1737,10 @@
         <v>66</v>
       </c>
       <c r="B19" t="s">
+        <v>297</v>
+      </c>
+      <c r="C19" s="6" t="s">
         <v>67</v>
-      </c>
-      <c r="C19" s="6" t="s">
-        <v>68</v>
       </c>
       <c r="D19" s="1"/>
       <c r="E19">
@@ -1745,42 +1748,47 @@
       </c>
       <c r="F19" s="1"/>
       <c r="G19" s="1"/>
-      <c r="H19" s="1"/>
+      <c r="H19" s="1" t="s">
+        <v>298</v>
+      </c>
       <c r="I19" s="1"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B20" t="s">
         <v>50</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="D20" s="6" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E20">
         <v>70983</v>
       </c>
-      <c r="F20" s="1"/>
-      <c r="G20" s="1"/>
-      <c r="H20" s="1"/>
+      <c r="F20" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>295</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>288</v>
+      </c>
       <c r="I20" s="1"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
+        <v>70</v>
+      </c>
+      <c r="B21" t="s">
+        <v>71</v>
+      </c>
+      <c r="C21" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="B21" t="s">
+      <c r="D21" s="6" t="s">
         <v>73</v>
-      </c>
-      <c r="C21" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="D21" s="6" t="s">
-        <v>75</v>
       </c>
       <c r="E21">
         <v>69484</v>
@@ -1792,13 +1800,13 @@
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
+        <v>74</v>
+      </c>
+      <c r="B22" t="s">
+        <v>75</v>
+      </c>
+      <c r="C22" s="6" t="s">
         <v>76</v>
-      </c>
-      <c r="B22" t="s">
-        <v>77</v>
-      </c>
-      <c r="C22" s="6" t="s">
-        <v>78</v>
       </c>
       <c r="D22" s="1"/>
       <c r="E22">
@@ -1811,13 +1819,13 @@
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B23" t="s">
         <v>19</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D23" s="1"/>
       <c r="E23">
@@ -1830,13 +1838,13 @@
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
+        <v>79</v>
+      </c>
+      <c r="B24" t="s">
+        <v>80</v>
+      </c>
+      <c r="C24" s="6" t="s">
         <v>81</v>
-      </c>
-      <c r="B24" t="s">
-        <v>82</v>
-      </c>
-      <c r="C24" s="6" t="s">
-        <v>83</v>
       </c>
       <c r="D24" s="1"/>
       <c r="E24">
@@ -1849,13 +1857,13 @@
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B25" t="s">
         <v>55</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D25" s="1"/>
       <c r="E25">
@@ -1868,13 +1876,13 @@
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
+        <v>84</v>
+      </c>
+      <c r="B26" t="s">
+        <v>85</v>
+      </c>
+      <c r="C26" s="6" t="s">
         <v>86</v>
-      </c>
-      <c r="B26" t="s">
-        <v>87</v>
-      </c>
-      <c r="C26" s="6" t="s">
-        <v>88</v>
       </c>
       <c r="E26">
         <v>60356</v>
@@ -1885,16 +1893,16 @@
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
+        <v>87</v>
+      </c>
+      <c r="B27" t="s">
+        <v>88</v>
+      </c>
+      <c r="C27" s="6" t="s">
         <v>89</v>
       </c>
-      <c r="B27" t="s">
+      <c r="D27" s="6" t="s">
         <v>90</v>
-      </c>
-      <c r="C27" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="D27" s="6" t="s">
-        <v>92</v>
       </c>
       <c r="E27">
         <v>60140</v>
@@ -1906,13 +1914,13 @@
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
+        <v>91</v>
+      </c>
+      <c r="B28" t="s">
+        <v>92</v>
+      </c>
+      <c r="C28" s="6" t="s">
         <v>93</v>
-      </c>
-      <c r="B28" t="s">
-        <v>94</v>
-      </c>
-      <c r="C28" s="6" t="s">
-        <v>95</v>
       </c>
       <c r="D28" s="1"/>
       <c r="E28">
@@ -1925,13 +1933,13 @@
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
+        <v>94</v>
+      </c>
+      <c r="B29" t="s">
+        <v>95</v>
+      </c>
+      <c r="C29" s="6" t="s">
         <v>96</v>
-      </c>
-      <c r="B29" t="s">
-        <v>97</v>
-      </c>
-      <c r="C29" s="6" t="s">
-        <v>98</v>
       </c>
       <c r="E29">
         <v>58698</v>
@@ -1942,13 +1950,13 @@
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
+        <v>97</v>
+      </c>
+      <c r="B30" t="s">
+        <v>98</v>
+      </c>
+      <c r="C30" s="6" t="s">
         <v>99</v>
-      </c>
-      <c r="B30" t="s">
-        <v>100</v>
-      </c>
-      <c r="C30" s="6" t="s">
-        <v>101</v>
       </c>
       <c r="D30" s="1"/>
       <c r="E30">
@@ -1961,13 +1969,13 @@
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
+        <v>100</v>
+      </c>
+      <c r="B31" t="s">
+        <v>101</v>
+      </c>
+      <c r="C31" s="6" t="s">
         <v>102</v>
-      </c>
-      <c r="B31" t="s">
-        <v>103</v>
-      </c>
-      <c r="C31" s="6" t="s">
-        <v>104</v>
       </c>
       <c r="D31" s="1"/>
       <c r="E31">
@@ -1980,13 +1988,13 @@
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B32" t="s">
         <v>19</v>
       </c>
       <c r="C32" s="6" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D32" s="1"/>
       <c r="E32">
@@ -1999,10 +2007,10 @@
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="E33">
         <v>55963</v>
@@ -2013,13 +2021,13 @@
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
+        <v>107</v>
+      </c>
+      <c r="B34" t="s">
+        <v>108</v>
+      </c>
+      <c r="C34" s="6" t="s">
         <v>109</v>
-      </c>
-      <c r="B34" t="s">
-        <v>110</v>
-      </c>
-      <c r="C34" s="6" t="s">
-        <v>111</v>
       </c>
       <c r="D34" s="1"/>
       <c r="E34">
@@ -2032,16 +2040,16 @@
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B35" t="s">
         <v>55</v>
       </c>
       <c r="C35" s="6" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D35" s="4" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="E35">
         <v>53282</v>
@@ -2053,13 +2061,13 @@
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B36" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C36" s="6" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D36" s="1"/>
       <c r="E36">
@@ -2072,13 +2080,13 @@
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
+        <v>115</v>
+      </c>
+      <c r="B37" t="s">
+        <v>116</v>
+      </c>
+      <c r="C37" s="6" t="s">
         <v>117</v>
-      </c>
-      <c r="B37" t="s">
-        <v>118</v>
-      </c>
-      <c r="C37" s="6" t="s">
-        <v>119</v>
       </c>
       <c r="D37" s="1"/>
       <c r="E37">
@@ -2091,16 +2099,16 @@
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
+        <v>118</v>
+      </c>
+      <c r="B38" t="s">
+        <v>119</v>
+      </c>
+      <c r="C38" s="6" t="s">
         <v>120</v>
       </c>
-      <c r="B38" t="s">
+      <c r="D38" s="6" t="s">
         <v>121</v>
-      </c>
-      <c r="C38" s="6" t="s">
-        <v>122</v>
-      </c>
-      <c r="D38" s="6" t="s">
-        <v>123</v>
       </c>
       <c r="E38">
         <v>50650</v>
@@ -2112,13 +2120,13 @@
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B39" t="s">
         <v>19</v>
       </c>
       <c r="C39" s="6" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D39" s="1"/>
       <c r="E39">
@@ -2131,16 +2139,16 @@
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
+        <v>124</v>
+      </c>
+      <c r="B40" t="s">
+        <v>125</v>
+      </c>
+      <c r="C40" s="6" t="s">
         <v>126</v>
       </c>
-      <c r="B40" t="s">
+      <c r="D40" s="4" t="s">
         <v>127</v>
-      </c>
-      <c r="C40" s="6" t="s">
-        <v>128</v>
-      </c>
-      <c r="D40" s="4" t="s">
-        <v>129</v>
       </c>
       <c r="E40">
         <v>50301</v>
@@ -2152,13 +2160,13 @@
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B41" t="s">
         <v>61</v>
       </c>
       <c r="C41" s="6" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="E41">
         <v>49974</v>
@@ -2169,13 +2177,13 @@
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B42" t="s">
         <v>61</v>
       </c>
       <c r="C42" s="6" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="D42" s="1"/>
       <c r="E42">
@@ -2188,13 +2196,13 @@
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B43" t="s">
         <v>64</v>
       </c>
       <c r="C43" s="6" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D43" s="1"/>
       <c r="E43">
@@ -2207,13 +2215,13 @@
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B44" t="s">
         <v>61</v>
       </c>
       <c r="C44" s="6" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="E44">
         <v>48271</v>
@@ -2224,13 +2232,13 @@
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
+        <v>136</v>
+      </c>
+      <c r="B45" t="s">
+        <v>137</v>
+      </c>
+      <c r="C45" s="6" t="s">
         <v>138</v>
-      </c>
-      <c r="B45" t="s">
-        <v>139</v>
-      </c>
-      <c r="C45" s="6" t="s">
-        <v>140</v>
       </c>
       <c r="D45" s="1"/>
       <c r="E45">
@@ -2243,13 +2251,13 @@
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B46" t="s">
         <v>61</v>
       </c>
       <c r="C46" s="6" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="D46" s="1"/>
       <c r="E46">
@@ -2259,23 +2267,23 @@
         <v>11</v>
       </c>
       <c r="G46" s="1" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="H46" s="1"/>
       <c r="I46" s="1"/>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
+        <v>141</v>
+      </c>
+      <c r="B47" t="s">
+        <v>142</v>
+      </c>
+      <c r="C47" s="6" t="s">
         <v>143</v>
       </c>
-      <c r="B47" t="s">
+      <c r="D47" s="6" t="s">
         <v>144</v>
-      </c>
-      <c r="C47" s="6" t="s">
-        <v>145</v>
-      </c>
-      <c r="D47" s="6" t="s">
-        <v>146</v>
       </c>
       <c r="E47">
         <v>46087</v>
@@ -2286,13 +2294,13 @@
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
+        <v>145</v>
+      </c>
+      <c r="B48" t="s">
+        <v>146</v>
+      </c>
+      <c r="C48" s="6" t="s">
         <v>147</v>
-      </c>
-      <c r="B48" t="s">
-        <v>148</v>
-      </c>
-      <c r="C48" s="6" t="s">
-        <v>149</v>
       </c>
       <c r="E48">
         <v>45189</v>
@@ -2303,16 +2311,16 @@
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B49" t="s">
         <v>55</v>
       </c>
       <c r="C49" s="6" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="D49" s="4" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="E49">
         <v>43716</v>
@@ -2324,13 +2332,13 @@
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
+        <v>151</v>
+      </c>
+      <c r="B50" s="7" t="s">
+        <v>152</v>
+      </c>
+      <c r="C50" s="6" t="s">
         <v>153</v>
-      </c>
-      <c r="B50" s="7" t="s">
-        <v>154</v>
-      </c>
-      <c r="C50" s="6" t="s">
-        <v>155</v>
       </c>
       <c r="D50" s="1"/>
       <c r="E50">
@@ -2343,13 +2351,13 @@
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B51" t="s">
         <v>55</v>
       </c>
       <c r="C51" s="6" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="D51" s="1"/>
       <c r="E51">
@@ -2362,13 +2370,13 @@
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C52" s="6" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="D52" s="1"/>
       <c r="E52">
@@ -2381,13 +2389,13 @@
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B53" t="s">
         <v>64</v>
       </c>
       <c r="C53" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="D53" s="1"/>
       <c r="E53">
@@ -2397,20 +2405,20 @@
         <v>11</v>
       </c>
       <c r="G53" s="9" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="H53" s="1"/>
       <c r="I53" s="1"/>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B54" t="s">
         <v>19</v>
       </c>
       <c r="C54" s="6" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="D54" s="1"/>
       <c r="E54">
@@ -2423,13 +2431,13 @@
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
+        <v>162</v>
+      </c>
+      <c r="B55" t="s">
+        <v>163</v>
+      </c>
+      <c r="C55" s="6" t="s">
         <v>164</v>
-      </c>
-      <c r="B55" t="s">
-        <v>165</v>
-      </c>
-      <c r="C55" s="6" t="s">
-        <v>166</v>
       </c>
       <c r="D55" s="1"/>
       <c r="E55">
@@ -2442,13 +2450,13 @@
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
+        <v>165</v>
+      </c>
+      <c r="B56" t="s">
+        <v>166</v>
+      </c>
+      <c r="C56" s="6" t="s">
         <v>167</v>
-      </c>
-      <c r="B56" t="s">
-        <v>168</v>
-      </c>
-      <c r="C56" s="6" t="s">
-        <v>169</v>
       </c>
       <c r="D56" s="1"/>
       <c r="E56">
@@ -2461,16 +2469,16 @@
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B57" t="s">
         <v>33</v>
       </c>
       <c r="C57" s="6" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="D57" s="6" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="E57">
         <v>41217</v>
@@ -2481,13 +2489,13 @@
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
+        <v>171</v>
+      </c>
+      <c r="B58" t="s">
+        <v>172</v>
+      </c>
+      <c r="C58" s="6" t="s">
         <v>173</v>
-      </c>
-      <c r="B58" t="s">
-        <v>174</v>
-      </c>
-      <c r="C58" s="6" t="s">
-        <v>175</v>
       </c>
       <c r="D58" s="1"/>
       <c r="E58">
@@ -2500,16 +2508,16 @@
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
+        <v>174</v>
+      </c>
+      <c r="B59" t="s">
+        <v>175</v>
+      </c>
+      <c r="C59" s="6" t="s">
         <v>176</v>
       </c>
-      <c r="B59" t="s">
+      <c r="D59" s="6" t="s">
         <v>177</v>
-      </c>
-      <c r="C59" s="6" t="s">
-        <v>178</v>
-      </c>
-      <c r="D59" s="6" t="s">
-        <v>179</v>
       </c>
       <c r="E59">
         <v>40911</v>
@@ -2521,13 +2529,13 @@
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
+        <v>178</v>
+      </c>
+      <c r="B60" t="s">
+        <v>179</v>
+      </c>
+      <c r="C60" s="6" t="s">
         <v>180</v>
-      </c>
-      <c r="B60" t="s">
-        <v>181</v>
-      </c>
-      <c r="C60" s="6" t="s">
-        <v>182</v>
       </c>
       <c r="D60" s="1"/>
       <c r="E60">
@@ -2540,13 +2548,13 @@
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
+        <v>181</v>
+      </c>
+      <c r="B61" t="s">
+        <v>182</v>
+      </c>
+      <c r="C61" s="6" t="s">
         <v>183</v>
-      </c>
-      <c r="B61" t="s">
-        <v>184</v>
-      </c>
-      <c r="C61" s="6" t="s">
-        <v>185</v>
       </c>
       <c r="D61" s="1"/>
       <c r="E61">
@@ -2559,13 +2567,13 @@
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
+        <v>184</v>
+      </c>
+      <c r="B62" t="s">
+        <v>185</v>
+      </c>
+      <c r="C62" s="6" t="s">
         <v>186</v>
-      </c>
-      <c r="B62" t="s">
-        <v>187</v>
-      </c>
-      <c r="C62" s="6" t="s">
-        <v>188</v>
       </c>
       <c r="D62" s="1"/>
       <c r="E62">
@@ -2578,16 +2586,16 @@
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
+        <v>187</v>
+      </c>
+      <c r="B63" t="s">
+        <v>188</v>
+      </c>
+      <c r="C63" s="6" t="s">
         <v>189</v>
       </c>
-      <c r="B63" t="s">
+      <c r="D63" s="6" t="s">
         <v>190</v>
-      </c>
-      <c r="C63" s="6" t="s">
-        <v>191</v>
-      </c>
-      <c r="D63" s="6" t="s">
-        <v>192</v>
       </c>
       <c r="E63">
         <v>38638</v>
@@ -2599,13 +2607,13 @@
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
+        <v>191</v>
+      </c>
+      <c r="B64" t="s">
+        <v>192</v>
+      </c>
+      <c r="C64" s="6" t="s">
         <v>193</v>
-      </c>
-      <c r="B64" t="s">
-        <v>194</v>
-      </c>
-      <c r="C64" s="6" t="s">
-        <v>195</v>
       </c>
       <c r="D64" s="1"/>
       <c r="E64">
@@ -2618,16 +2626,16 @@
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
+        <v>194</v>
+      </c>
+      <c r="B65" t="s">
+        <v>195</v>
+      </c>
+      <c r="C65" s="6" t="s">
         <v>196</v>
       </c>
-      <c r="B65" t="s">
+      <c r="D65" s="6" t="s">
         <v>197</v>
-      </c>
-      <c r="C65" s="6" t="s">
-        <v>198</v>
-      </c>
-      <c r="D65" s="6" t="s">
-        <v>199</v>
       </c>
       <c r="E65">
         <v>38197</v>
@@ -2638,13 +2646,13 @@
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
+        <v>198</v>
+      </c>
+      <c r="B66" s="5" t="s">
+        <v>199</v>
+      </c>
+      <c r="C66" s="6" t="s">
         <v>200</v>
-      </c>
-      <c r="B66" s="5" t="s">
-        <v>201</v>
-      </c>
-      <c r="C66" s="6" t="s">
-        <v>202</v>
       </c>
       <c r="D66" s="1"/>
       <c r="E66">
@@ -2657,13 +2665,13 @@
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
+        <v>201</v>
+      </c>
+      <c r="B67" t="s">
+        <v>202</v>
+      </c>
+      <c r="C67" s="6" t="s">
         <v>203</v>
-      </c>
-      <c r="B67" t="s">
-        <v>204</v>
-      </c>
-      <c r="C67" s="6" t="s">
-        <v>205</v>
       </c>
       <c r="D67" s="1"/>
       <c r="E67">
@@ -2676,13 +2684,13 @@
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="B68" t="s">
         <v>55</v>
       </c>
       <c r="C68" s="6" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="D68" s="1"/>
       <c r="E68">
@@ -2695,13 +2703,13 @@
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="B69" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C69" s="6" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="E69">
         <v>36139</v>
@@ -2712,13 +2720,13 @@
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="B70" t="s">
         <v>61</v>
       </c>
       <c r="C70" s="6" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="D70" s="1"/>
       <c r="E70">
@@ -2731,13 +2739,13 @@
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="B71" t="s">
         <v>30</v>
       </c>
       <c r="C71" s="6" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="D71" s="1"/>
       <c r="E71">
@@ -2750,13 +2758,13 @@
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="B72" t="s">
         <v>61</v>
       </c>
       <c r="C72" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="D72" s="1"/>
       <c r="E72">
@@ -2766,20 +2774,20 @@
         <v>11</v>
       </c>
       <c r="G72" s="1" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="H72" s="1"/>
       <c r="I72" s="1"/>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
+        <v>214</v>
+      </c>
+      <c r="B73" t="s">
+        <v>215</v>
+      </c>
+      <c r="C73" s="6" t="s">
         <v>216</v>
-      </c>
-      <c r="B73" t="s">
-        <v>217</v>
-      </c>
-      <c r="C73" s="6" t="s">
-        <v>218</v>
       </c>
       <c r="D73" s="1"/>
       <c r="E73">
@@ -2792,13 +2800,13 @@
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="B74" t="s">
         <v>55</v>
       </c>
       <c r="C74" s="6" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="D74" s="1"/>
       <c r="E74">
@@ -2811,16 +2819,16 @@
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="B75" t="s">
         <v>30</v>
       </c>
       <c r="C75" s="6" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="D75" s="6" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="E75">
         <v>29827</v>
@@ -2831,13 +2839,13 @@
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B76" t="s">
         <v>61</v>
       </c>
       <c r="C76" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="D76" s="1"/>
       <c r="E76">
@@ -2847,23 +2855,23 @@
         <v>11</v>
       </c>
       <c r="G76" s="1" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="H76" s="9"/>
       <c r="I76" s="1"/>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
+        <v>224</v>
+      </c>
+      <c r="B77" t="s">
+        <v>225</v>
+      </c>
+      <c r="C77" s="6" t="s">
         <v>226</v>
       </c>
-      <c r="B77" t="s">
+      <c r="D77" s="6" t="s">
         <v>227</v>
-      </c>
-      <c r="C77" s="6" t="s">
-        <v>228</v>
-      </c>
-      <c r="D77" s="6" t="s">
-        <v>229</v>
       </c>
       <c r="E77">
         <v>29516</v>
@@ -2875,10 +2883,10 @@
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="B78" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="D78" s="1"/>
       <c r="E78">
@@ -2891,16 +2899,16 @@
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="B79" t="s">
         <v>33</v>
       </c>
       <c r="C79" s="6" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="D79" s="6" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="E79">
         <v>27743</v>
@@ -2912,13 +2920,13 @@
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
+        <v>233</v>
+      </c>
+      <c r="B80" t="s">
+        <v>234</v>
+      </c>
+      <c r="C80" s="6" t="s">
         <v>235</v>
-      </c>
-      <c r="B80" t="s">
-        <v>236</v>
-      </c>
-      <c r="C80" s="6" t="s">
-        <v>237</v>
       </c>
       <c r="D80" s="1"/>
       <c r="E80">
@@ -2931,13 +2939,13 @@
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="B81" t="s">
         <v>19</v>
       </c>
       <c r="C81" s="6" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="D81" s="1"/>
       <c r="E81">
@@ -2950,13 +2958,13 @@
     </row>
     <row r="82" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
+        <v>238</v>
+      </c>
+      <c r="B82" s="3" t="s">
+        <v>239</v>
+      </c>
+      <c r="C82" s="6" t="s">
         <v>240</v>
-      </c>
-      <c r="B82" s="3" t="s">
-        <v>241</v>
-      </c>
-      <c r="C82" s="6" t="s">
-        <v>242</v>
       </c>
       <c r="D82" s="1"/>
       <c r="E82">
@@ -2969,13 +2977,13 @@
     </row>
     <row r="83" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
+        <v>241</v>
+      </c>
+      <c r="B83" t="s">
+        <v>242</v>
+      </c>
+      <c r="C83" s="6" t="s">
         <v>243</v>
-      </c>
-      <c r="B83" t="s">
-        <v>244</v>
-      </c>
-      <c r="C83" s="6" t="s">
-        <v>245</v>
       </c>
       <c r="E83">
         <v>25028</v>
@@ -2986,13 +2994,13 @@
     </row>
     <row r="84" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
+        <v>244</v>
+      </c>
+      <c r="B84" t="s">
+        <v>245</v>
+      </c>
+      <c r="C84" s="6" t="s">
         <v>246</v>
-      </c>
-      <c r="B84" t="s">
-        <v>247</v>
-      </c>
-      <c r="C84" s="6" t="s">
-        <v>248</v>
       </c>
       <c r="D84" s="1"/>
       <c r="E84">
@@ -3005,16 +3013,16 @@
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
+        <v>247</v>
+      </c>
+      <c r="B85" t="s">
+        <v>248</v>
+      </c>
+      <c r="C85" s="6" t="s">
         <v>249</v>
       </c>
-      <c r="B85" t="s">
+      <c r="D85" s="6" t="s">
         <v>250</v>
-      </c>
-      <c r="C85" s="6" t="s">
-        <v>251</v>
-      </c>
-      <c r="D85" s="6" t="s">
-        <v>252</v>
       </c>
       <c r="E85">
         <v>22988</v>
@@ -3025,13 +3033,13 @@
     </row>
     <row r="86" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
+        <v>251</v>
+      </c>
+      <c r="B86" t="s">
+        <v>252</v>
+      </c>
+      <c r="C86" s="6" t="s">
         <v>253</v>
-      </c>
-      <c r="B86" t="s">
-        <v>254</v>
-      </c>
-      <c r="C86" s="6" t="s">
-        <v>255</v>
       </c>
       <c r="D86" s="1"/>
       <c r="E86">
@@ -3044,13 +3052,13 @@
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="B87" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C87" s="6" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="D87" s="1"/>
       <c r="E87">
@@ -3063,13 +3071,13 @@
     </row>
     <row r="88" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
+        <v>256</v>
+      </c>
+      <c r="B88" t="s">
+        <v>257</v>
+      </c>
+      <c r="C88" s="6" t="s">
         <v>258</v>
-      </c>
-      <c r="B88" t="s">
-        <v>259</v>
-      </c>
-      <c r="C88" s="6" t="s">
-        <v>260</v>
       </c>
       <c r="D88" s="1"/>
       <c r="E88">
@@ -3082,13 +3090,13 @@
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="B89" t="s">
         <v>55</v>
       </c>
       <c r="C89" s="6" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="D89" s="1"/>
       <c r="E89">
@@ -3101,13 +3109,13 @@
     </row>
     <row r="90" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
+        <v>261</v>
+      </c>
+      <c r="B90" t="s">
+        <v>262</v>
+      </c>
+      <c r="C90" s="6" t="s">
         <v>263</v>
-      </c>
-      <c r="B90" t="s">
-        <v>264</v>
-      </c>
-      <c r="C90" s="6" t="s">
-        <v>265</v>
       </c>
       <c r="D90" s="1"/>
       <c r="E90">
@@ -3120,13 +3128,13 @@
     </row>
     <row r="91" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="B91" t="s">
         <v>61</v>
       </c>
       <c r="C91" s="6" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="E91">
         <v>20514</v>
@@ -3137,13 +3145,13 @@
     </row>
     <row r="92" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
+        <v>266</v>
+      </c>
+      <c r="B92" t="s">
+        <v>267</v>
+      </c>
+      <c r="C92" s="6" t="s">
         <v>268</v>
-      </c>
-      <c r="B92" t="s">
-        <v>269</v>
-      </c>
-      <c r="C92" s="6" t="s">
-        <v>270</v>
       </c>
       <c r="E92">
         <v>20133</v>
@@ -3154,13 +3162,13 @@
     </row>
     <row r="93" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
+        <v>269</v>
+      </c>
+      <c r="B93" t="s">
+        <v>270</v>
+      </c>
+      <c r="C93" s="6" t="s">
         <v>271</v>
-      </c>
-      <c r="B93" t="s">
-        <v>272</v>
-      </c>
-      <c r="C93" s="6" t="s">
-        <v>273</v>
       </c>
       <c r="D93" s="1"/>
       <c r="E93">
@@ -3173,13 +3181,13 @@
     </row>
     <row r="94" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="B94" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C94" s="6" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="E94">
         <v>14272</v>
@@ -3190,13 +3198,13 @@
     </row>
     <row r="95" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="B95" t="s">
         <v>55</v>
       </c>
       <c r="C95" s="6" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="D95" s="1"/>
       <c r="E95">
@@ -3209,13 +3217,13 @@
     </row>
     <row r="96" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="B96" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="C96" s="6" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="E96">
         <v>6178</v>
@@ -3226,13 +3234,13 @@
     </row>
     <row r="97" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="B97" t="s">
         <v>61</v>
       </c>
       <c r="C97" s="6" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="D97" s="1"/>
       <c r="E97">
@@ -3242,20 +3250,20 @@
         <v>11</v>
       </c>
       <c r="G97" s="1" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="H97" s="8"/>
       <c r="I97" s="1"/>
     </row>
     <row r="98" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="B98" t="s">
         <v>61</v>
       </c>
       <c r="C98" s="6" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="E98">
         <v>3401</v>
@@ -3264,18 +3272,18 @@
         <v>11</v>
       </c>
       <c r="G98" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
     </row>
     <row r="99" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
+        <v>282</v>
+      </c>
+      <c r="B99" t="s">
+        <v>283</v>
+      </c>
+      <c r="C99" s="6" t="s">
         <v>284</v>
-      </c>
-      <c r="B99" t="s">
-        <v>285</v>
-      </c>
-      <c r="C99" s="6" t="s">
-        <v>286</v>
       </c>
       <c r="E99">
         <v>1807</v>
@@ -3328,77 +3336,76 @@
     <hyperlink ref="D38" r:id="rId40" xr:uid="{00000000-0004-0000-0000-000027000000}"/>
     <hyperlink ref="C38" r:id="rId41" xr:uid="{00000000-0004-0000-0000-000028000000}"/>
     <hyperlink ref="C22" r:id="rId42" xr:uid="{00000000-0004-0000-0000-000029000000}"/>
-    <hyperlink ref="C20" r:id="rId43" xr:uid="{00000000-0004-0000-0000-00002A000000}"/>
-    <hyperlink ref="D20" r:id="rId44" xr:uid="{00000000-0004-0000-0000-00002B000000}"/>
-    <hyperlink ref="C30" r:id="rId45" xr:uid="{00000000-0004-0000-0000-00002C000000}"/>
-    <hyperlink ref="C13" r:id="rId46" xr:uid="{00000000-0004-0000-0000-00002D000000}"/>
-    <hyperlink ref="D35" r:id="rId47" xr:uid="{00000000-0004-0000-0000-00002E000000}"/>
-    <hyperlink ref="C35" r:id="rId48" xr:uid="{00000000-0004-0000-0000-00002F000000}"/>
-    <hyperlink ref="C39" r:id="rId49" xr:uid="{00000000-0004-0000-0000-000030000000}"/>
-    <hyperlink ref="C83" r:id="rId50" xr:uid="{00000000-0004-0000-0000-000031000000}"/>
-    <hyperlink ref="C58" r:id="rId51" xr:uid="{00000000-0004-0000-0000-000032000000}"/>
-    <hyperlink ref="C85" r:id="rId52" xr:uid="{00000000-0004-0000-0000-000033000000}"/>
-    <hyperlink ref="D85" r:id="rId53" xr:uid="{00000000-0004-0000-0000-000034000000}"/>
-    <hyperlink ref="C63" r:id="rId54" xr:uid="{00000000-0004-0000-0000-000035000000}"/>
-    <hyperlink ref="D63" r:id="rId55" xr:uid="{00000000-0004-0000-0000-000036000000}"/>
-    <hyperlink ref="C42" r:id="rId56" xr:uid="{00000000-0004-0000-0000-000037000000}"/>
-    <hyperlink ref="C84" r:id="rId57" xr:uid="{00000000-0004-0000-0000-000038000000}"/>
-    <hyperlink ref="C11" r:id="rId58" xr:uid="{00000000-0004-0000-0000-000039000000}"/>
-    <hyperlink ref="D11" r:id="rId59" xr:uid="{00000000-0004-0000-0000-00003A000000}"/>
-    <hyperlink ref="C95" r:id="rId60" xr:uid="{00000000-0004-0000-0000-00003B000000}"/>
-    <hyperlink ref="C80" r:id="rId61" xr:uid="{00000000-0004-0000-0000-00003C000000}"/>
-    <hyperlink ref="C92" r:id="rId62" xr:uid="{00000000-0004-0000-0000-00003D000000}"/>
-    <hyperlink ref="C91" r:id="rId63" xr:uid="{00000000-0004-0000-0000-00003E000000}"/>
-    <hyperlink ref="C65" r:id="rId64" xr:uid="{00000000-0004-0000-0000-00003F000000}"/>
-    <hyperlink ref="D65" r:id="rId65" display="http://polweb.norddjurs.dk/Arkiv Politiske Udvalg/Forms/AllItems.aspx?" xr:uid="{00000000-0004-0000-0000-000040000000}"/>
-    <hyperlink ref="D77" r:id="rId66" xr:uid="{00000000-0004-0000-0000-000041000000}"/>
-    <hyperlink ref="C77" r:id="rId67" xr:uid="{00000000-0004-0000-0000-000042000000}"/>
-    <hyperlink ref="C16" r:id="rId68" display="https://www.naestved.dk/ByraadPolitik/Dagsordenerogreferater/Se dagsordener og referater her.aspx" xr:uid="{00000000-0004-0000-0000-000043000000}"/>
-    <hyperlink ref="D16" r:id="rId69" xr:uid="{00000000-0004-0000-0000-000044000000}"/>
-    <hyperlink ref="C73" r:id="rId70" xr:uid="{00000000-0004-0000-0000-000045000000}"/>
-    <hyperlink ref="C88" r:id="rId71" xr:uid="{00000000-0004-0000-0000-000046000000}"/>
-    <hyperlink ref="C26" r:id="rId72" xr:uid="{00000000-0004-0000-0000-000047000000}"/>
-    <hyperlink ref="C55" r:id="rId73" xr:uid="{00000000-0004-0000-0000-000048000000}"/>
-    <hyperlink ref="C34" r:id="rId74" xr:uid="{00000000-0004-0000-0000-000049000000}"/>
-    <hyperlink ref="C99" r:id="rId75" xr:uid="{00000000-0004-0000-0000-00004A000000}"/>
-    <hyperlink ref="C54" r:id="rId76" xr:uid="{00000000-0004-0000-0000-00004B000000}"/>
-    <hyperlink ref="C64" r:id="rId77" display="https://www.middelfart.dk/Politik og demokrati/Byraad 2014/Referater 2014 til 2017" xr:uid="{00000000-0004-0000-0000-00004C000000}"/>
-    <hyperlink ref="C9" r:id="rId78" xr:uid="{00000000-0004-0000-0000-00004D000000}"/>
-    <hyperlink ref="C75" r:id="rId79" xr:uid="{00000000-0004-0000-0000-00004E000000}"/>
-    <hyperlink ref="D75" r:id="rId80" xr:uid="{00000000-0004-0000-0000-00004F000000}"/>
-    <hyperlink ref="C31" r:id="rId81" xr:uid="{00000000-0004-0000-0000-000050000000}"/>
-    <hyperlink ref="C71" r:id="rId82" xr:uid="{00000000-0004-0000-0000-000051000000}"/>
-    <hyperlink ref="C15" r:id="rId83" xr:uid="{00000000-0004-0000-0000-000052000000}"/>
-    <hyperlink ref="C32" r:id="rId84" xr:uid="{00000000-0004-0000-0000-000053000000}"/>
-    <hyperlink ref="C62" r:id="rId85" xr:uid="{00000000-0004-0000-0000-000054000000}"/>
-    <hyperlink ref="C12" r:id="rId86" xr:uid="{00000000-0004-0000-0000-000055000000}"/>
-    <hyperlink ref="C25" r:id="rId87" xr:uid="{00000000-0004-0000-0000-000056000000}"/>
-    <hyperlink ref="C17" r:id="rId88" xr:uid="{00000000-0004-0000-0000-000057000000}"/>
-    <hyperlink ref="C89" r:id="rId89" xr:uid="{00000000-0004-0000-0000-000058000000}"/>
-    <hyperlink ref="C86" r:id="rId90" xr:uid="{00000000-0004-0000-0000-000059000000}"/>
-    <hyperlink ref="C90" r:id="rId91" xr:uid="{00000000-0004-0000-0000-00005A000000}"/>
-    <hyperlink ref="C29" r:id="rId92" xr:uid="{00000000-0004-0000-0000-00005B000000}"/>
-    <hyperlink ref="C19" r:id="rId93" xr:uid="{00000000-0004-0000-0000-00005C000000}"/>
-    <hyperlink ref="C49" r:id="rId94" xr:uid="{00000000-0004-0000-0000-00005D000000}"/>
-    <hyperlink ref="D49" r:id="rId95" xr:uid="{00000000-0004-0000-0000-00005E000000}"/>
-    <hyperlink ref="C50" r:id="rId96" xr:uid="{00000000-0004-0000-0000-00005F000000}"/>
-    <hyperlink ref="C66" r:id="rId97" xr:uid="{00000000-0004-0000-0000-000060000000}"/>
-    <hyperlink ref="C2" r:id="rId98" display="https://www.kk.dk/dagsordener-og-referater?field_committee_type_tid%5B%5D=13957&amp;field_committee_type_tid%5B%5D=13960&amp;field_committee_type_tid%5B%5D=13959&amp;field_committee_type_tid%5B%5D=13958&amp;title=&amp;field_date_single_value%5Bvalue%5D%5Bdate%5D=01.01.2007&amp;field_date_single_value_1%5Bvalue%5D%5Bdate%5D=01.01.2018" xr:uid="{00000000-0004-0000-0000-000061000000}"/>
-    <hyperlink ref="C93" r:id="rId99" display="https://www.vallensbaek.dk/kommunen/dagsordner-og-referater/dagsordner-og-referater?meetings_date_from%5Bvalue%5D%5Bmonth%5D=7&amp;meetings_date_from%5Bvalue%5D%5Byear%5D=2013&amp;meetings_to_date%5Bvalue%5D%5Bmonth%5D=7&amp;meetings_to_date%5Bvalue%5D%5Byear%5D=2019&amp;field_os2web_meetings_committee_tid=All" xr:uid="{00000000-0004-0000-0000-000062000000}"/>
-    <hyperlink ref="C40" r:id="rId100" xr:uid="{00000000-0004-0000-0000-000063000000}"/>
-    <hyperlink ref="D40" r:id="rId101" xr:uid="{00000000-0004-0000-0000-000064000000}"/>
-    <hyperlink ref="C52" r:id="rId102" xr:uid="{00000000-0004-0000-0000-000065000000}"/>
-    <hyperlink ref="C7" r:id="rId103" xr:uid="{00000000-0004-0000-0000-000066000000}"/>
-    <hyperlink ref="C67" r:id="rId104" xr:uid="{00000000-0004-0000-0000-000067000000}"/>
-    <hyperlink ref="C10" r:id="rId105" xr:uid="{00000000-0004-0000-0000-000068000000}"/>
-    <hyperlink ref="D10" r:id="rId106" xr:uid="{00000000-0004-0000-0000-000069000000}"/>
-    <hyperlink ref="C47" r:id="rId107" xr:uid="{00000000-0004-0000-0000-00006A000000}"/>
-    <hyperlink ref="D47" r:id="rId108" xr:uid="{00000000-0004-0000-0000-00006B000000}"/>
-    <hyperlink ref="C96" r:id="rId109" xr:uid="{00000000-0004-0000-0000-00006C000000}"/>
-    <hyperlink ref="C4" r:id="rId110" xr:uid="{00000000-0004-0000-0000-00006D000000}"/>
-    <hyperlink ref="C5" r:id="rId111" xr:uid="{00000000-0004-0000-0000-00006E000000}"/>
+    <hyperlink ref="C20" r:id="rId43" xr:uid="{00000000-0004-0000-0000-00002B000000}"/>
+    <hyperlink ref="C30" r:id="rId44" xr:uid="{00000000-0004-0000-0000-00002C000000}"/>
+    <hyperlink ref="C13" r:id="rId45" xr:uid="{00000000-0004-0000-0000-00002D000000}"/>
+    <hyperlink ref="D35" r:id="rId46" xr:uid="{00000000-0004-0000-0000-00002E000000}"/>
+    <hyperlink ref="C35" r:id="rId47" xr:uid="{00000000-0004-0000-0000-00002F000000}"/>
+    <hyperlink ref="C39" r:id="rId48" xr:uid="{00000000-0004-0000-0000-000030000000}"/>
+    <hyperlink ref="C83" r:id="rId49" xr:uid="{00000000-0004-0000-0000-000031000000}"/>
+    <hyperlink ref="C58" r:id="rId50" xr:uid="{00000000-0004-0000-0000-000032000000}"/>
+    <hyperlink ref="C85" r:id="rId51" xr:uid="{00000000-0004-0000-0000-000033000000}"/>
+    <hyperlink ref="D85" r:id="rId52" xr:uid="{00000000-0004-0000-0000-000034000000}"/>
+    <hyperlink ref="C63" r:id="rId53" xr:uid="{00000000-0004-0000-0000-000035000000}"/>
+    <hyperlink ref="D63" r:id="rId54" xr:uid="{00000000-0004-0000-0000-000036000000}"/>
+    <hyperlink ref="C42" r:id="rId55" xr:uid="{00000000-0004-0000-0000-000037000000}"/>
+    <hyperlink ref="C84" r:id="rId56" xr:uid="{00000000-0004-0000-0000-000038000000}"/>
+    <hyperlink ref="C11" r:id="rId57" xr:uid="{00000000-0004-0000-0000-000039000000}"/>
+    <hyperlink ref="D11" r:id="rId58" xr:uid="{00000000-0004-0000-0000-00003A000000}"/>
+    <hyperlink ref="C95" r:id="rId59" xr:uid="{00000000-0004-0000-0000-00003B000000}"/>
+    <hyperlink ref="C80" r:id="rId60" xr:uid="{00000000-0004-0000-0000-00003C000000}"/>
+    <hyperlink ref="C92" r:id="rId61" xr:uid="{00000000-0004-0000-0000-00003D000000}"/>
+    <hyperlink ref="C91" r:id="rId62" xr:uid="{00000000-0004-0000-0000-00003E000000}"/>
+    <hyperlink ref="C65" r:id="rId63" xr:uid="{00000000-0004-0000-0000-00003F000000}"/>
+    <hyperlink ref="D65" r:id="rId64" display="http://polweb.norddjurs.dk/Arkiv Politiske Udvalg/Forms/AllItems.aspx?" xr:uid="{00000000-0004-0000-0000-000040000000}"/>
+    <hyperlink ref="D77" r:id="rId65" xr:uid="{00000000-0004-0000-0000-000041000000}"/>
+    <hyperlink ref="C77" r:id="rId66" xr:uid="{00000000-0004-0000-0000-000042000000}"/>
+    <hyperlink ref="C16" r:id="rId67" display="https://www.naestved.dk/ByraadPolitik/Dagsordenerogreferater/Se dagsordener og referater her.aspx" xr:uid="{00000000-0004-0000-0000-000043000000}"/>
+    <hyperlink ref="D16" r:id="rId68" xr:uid="{00000000-0004-0000-0000-000044000000}"/>
+    <hyperlink ref="C73" r:id="rId69" xr:uid="{00000000-0004-0000-0000-000045000000}"/>
+    <hyperlink ref="C88" r:id="rId70" xr:uid="{00000000-0004-0000-0000-000046000000}"/>
+    <hyperlink ref="C26" r:id="rId71" xr:uid="{00000000-0004-0000-0000-000047000000}"/>
+    <hyperlink ref="C55" r:id="rId72" xr:uid="{00000000-0004-0000-0000-000048000000}"/>
+    <hyperlink ref="C34" r:id="rId73" xr:uid="{00000000-0004-0000-0000-000049000000}"/>
+    <hyperlink ref="C99" r:id="rId74" xr:uid="{00000000-0004-0000-0000-00004A000000}"/>
+    <hyperlink ref="C54" r:id="rId75" xr:uid="{00000000-0004-0000-0000-00004B000000}"/>
+    <hyperlink ref="C64" r:id="rId76" display="https://www.middelfart.dk/Politik og demokrati/Byraad 2014/Referater 2014 til 2017" xr:uid="{00000000-0004-0000-0000-00004C000000}"/>
+    <hyperlink ref="C9" r:id="rId77" xr:uid="{00000000-0004-0000-0000-00004D000000}"/>
+    <hyperlink ref="C75" r:id="rId78" xr:uid="{00000000-0004-0000-0000-00004E000000}"/>
+    <hyperlink ref="D75" r:id="rId79" xr:uid="{00000000-0004-0000-0000-00004F000000}"/>
+    <hyperlink ref="C31" r:id="rId80" xr:uid="{00000000-0004-0000-0000-000050000000}"/>
+    <hyperlink ref="C71" r:id="rId81" xr:uid="{00000000-0004-0000-0000-000051000000}"/>
+    <hyperlink ref="C15" r:id="rId82" xr:uid="{00000000-0004-0000-0000-000052000000}"/>
+    <hyperlink ref="C32" r:id="rId83" xr:uid="{00000000-0004-0000-0000-000053000000}"/>
+    <hyperlink ref="C62" r:id="rId84" xr:uid="{00000000-0004-0000-0000-000054000000}"/>
+    <hyperlink ref="C12" r:id="rId85" xr:uid="{00000000-0004-0000-0000-000055000000}"/>
+    <hyperlink ref="C25" r:id="rId86" xr:uid="{00000000-0004-0000-0000-000056000000}"/>
+    <hyperlink ref="C17" r:id="rId87" xr:uid="{00000000-0004-0000-0000-000057000000}"/>
+    <hyperlink ref="C89" r:id="rId88" xr:uid="{00000000-0004-0000-0000-000058000000}"/>
+    <hyperlink ref="C86" r:id="rId89" xr:uid="{00000000-0004-0000-0000-000059000000}"/>
+    <hyperlink ref="C90" r:id="rId90" xr:uid="{00000000-0004-0000-0000-00005A000000}"/>
+    <hyperlink ref="C29" r:id="rId91" xr:uid="{00000000-0004-0000-0000-00005B000000}"/>
+    <hyperlink ref="C19" r:id="rId92" xr:uid="{00000000-0004-0000-0000-00005C000000}"/>
+    <hyperlink ref="C49" r:id="rId93" xr:uid="{00000000-0004-0000-0000-00005D000000}"/>
+    <hyperlink ref="D49" r:id="rId94" xr:uid="{00000000-0004-0000-0000-00005E000000}"/>
+    <hyperlink ref="C50" r:id="rId95" xr:uid="{00000000-0004-0000-0000-00005F000000}"/>
+    <hyperlink ref="C66" r:id="rId96" xr:uid="{00000000-0004-0000-0000-000060000000}"/>
+    <hyperlink ref="C2" r:id="rId97" display="https://www.kk.dk/dagsordener-og-referater?field_committee_type_tid%5B%5D=13957&amp;field_committee_type_tid%5B%5D=13960&amp;field_committee_type_tid%5B%5D=13959&amp;field_committee_type_tid%5B%5D=13958&amp;title=&amp;field_date_single_value%5Bvalue%5D%5Bdate%5D=01.01.2007&amp;field_date_single_value_1%5Bvalue%5D%5Bdate%5D=01.01.2018" xr:uid="{00000000-0004-0000-0000-000061000000}"/>
+    <hyperlink ref="C93" r:id="rId98" display="https://www.vallensbaek.dk/kommunen/dagsordner-og-referater/dagsordner-og-referater?meetings_date_from%5Bvalue%5D%5Bmonth%5D=7&amp;meetings_date_from%5Bvalue%5D%5Byear%5D=2013&amp;meetings_to_date%5Bvalue%5D%5Bmonth%5D=7&amp;meetings_to_date%5Bvalue%5D%5Byear%5D=2019&amp;field_os2web_meetings_committee_tid=All" xr:uid="{00000000-0004-0000-0000-000062000000}"/>
+    <hyperlink ref="C40" r:id="rId99" xr:uid="{00000000-0004-0000-0000-000063000000}"/>
+    <hyperlink ref="D40" r:id="rId100" xr:uid="{00000000-0004-0000-0000-000064000000}"/>
+    <hyperlink ref="C52" r:id="rId101" xr:uid="{00000000-0004-0000-0000-000065000000}"/>
+    <hyperlink ref="C7" r:id="rId102" xr:uid="{00000000-0004-0000-0000-000066000000}"/>
+    <hyperlink ref="C67" r:id="rId103" xr:uid="{00000000-0004-0000-0000-000067000000}"/>
+    <hyperlink ref="C10" r:id="rId104" xr:uid="{00000000-0004-0000-0000-000068000000}"/>
+    <hyperlink ref="D10" r:id="rId105" xr:uid="{00000000-0004-0000-0000-000069000000}"/>
+    <hyperlink ref="C47" r:id="rId106" xr:uid="{00000000-0004-0000-0000-00006A000000}"/>
+    <hyperlink ref="D47" r:id="rId107" xr:uid="{00000000-0004-0000-0000-00006B000000}"/>
+    <hyperlink ref="C96" r:id="rId108" xr:uid="{00000000-0004-0000-0000-00006C000000}"/>
+    <hyperlink ref="C4" r:id="rId109" xr:uid="{00000000-0004-0000-0000-00006D000000}"/>
+    <hyperlink ref="C5" r:id="rId110" xr:uid="{00000000-0004-0000-0000-00006E000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId112"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId111"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Finished the Helsingør scraper
</commit_message>
<xml_diff>
--- a/Kommuner.xlsx
+++ b/Kommuner.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\musse\OneDrive\UNI\9. semester\GitHub\First_Repository_CROW_FAR\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="45" documentId="11_FDF7A8DB94275223C5388096340570E2CE8365A4" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{7E213A68-37F6-49AB-804B-4153D0CF771A}"/>
+  <xr:revisionPtr revIDLastSave="46" documentId="11_FDF7A8DB94275223C5388096340570E2CE8365A4" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{497D500D-3EE4-4823-A204-D2E43DF3D4F4}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="300">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="299">
   <si>
     <t>Kommuner</t>
   </si>
@@ -916,9 +916,6 @@
   </si>
   <si>
     <t>2009 - 2017</t>
-  </si>
-  <si>
-    <t>Started</t>
   </si>
   <si>
     <t>2013 - 2017</t>
@@ -1319,8 +1316,8 @@
   <dimension ref="A1:I99"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G16" sqref="G16"/>
+      <pane ySplit="1" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1728,7 +1725,7 @@
         <v>11</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="H18" s="1" t="s">
         <v>285</v>
@@ -1841,10 +1838,10 @@
         <v>11</v>
       </c>
       <c r="G23" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H23" s="1" t="s">
         <v>297</v>
-      </c>
-      <c r="H23" s="1" t="s">
-        <v>298</v>
       </c>
       <c r="I23" s="1"/>
     </row>

</xml_diff>

<commit_message>
Created scraper for Køge
</commit_message>
<xml_diff>
--- a/Kommuner.xlsx
+++ b/Kommuner.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\musse\OneDrive\UNI\9. semester\GitHub\First_Repository_CROW_FAR\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="51" documentId="11_FDF7A8DB94275223C5388096340570E2CE8365A4" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{045F6A68-ED7D-4AC4-908F-40716783E1F0}"/>
+  <xr:revisionPtr revIDLastSave="55" documentId="11_FDF7A8DB94275223C5388096340570E2CE8365A4" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{0E86086F-83CA-41B2-B2BB-3FD8188F0155}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="371" uniqueCount="299">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="374" uniqueCount="299">
   <si>
     <t>Kommuner</t>
   </si>
@@ -1317,7 +1317,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G25" sqref="G25"/>
+      <selection pane="bottomLeft" activeCell="H26" sqref="H26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1875,7 +1875,7 @@
         <v>81</v>
       </c>
       <c r="B25" t="s">
-        <v>55</v>
+        <v>289</v>
       </c>
       <c r="C25" s="6" t="s">
         <v>82</v>
@@ -1902,8 +1902,15 @@
       <c r="E26">
         <v>60356</v>
       </c>
-      <c r="G26" s="1"/>
-      <c r="H26" s="1"/>
+      <c r="F26" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H26" s="1" t="s">
+        <v>287</v>
+      </c>
       <c r="I26" s="1"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Scraper for Frederikshavn done
</commit_message>
<xml_diff>
--- a/Kommuner.xlsx
+++ b/Kommuner.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\musse\OneDrive\UNI\9. semester\GitHub\First_Repository_CROW_FAR\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="55" documentId="11_FDF7A8DB94275223C5388096340570E2CE8365A4" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{0E86086F-83CA-41B2-B2BB-3FD8188F0155}"/>
+  <xr:revisionPtr revIDLastSave="62" documentId="11_FDF7A8DB94275223C5388096340570E2CE8365A4" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{3AC6DC05-7FC6-4537-815E-C5EC3501884E}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="374" uniqueCount="299">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="301">
   <si>
     <t>Kommuner</t>
   </si>
@@ -922,13 +922,31 @@
   </si>
   <si>
     <t>Files downloaded, not parsed though as items were not readily available</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">2007 - </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>2016</t>
+    </r>
+  </si>
+  <si>
+    <t>Done - 2017 is hidden behind java, maybe to be done later. Also not parsed into items, but by meeting. No items available.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -955,6 +973,13 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -987,7 +1012,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -998,6 +1023,18 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
@@ -1316,8 +1353,8 @@
   <dimension ref="A1:I99"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H26" sqref="H26"/>
+      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1327,7 +1364,7 @@
     <col min="3" max="3" width="32.453125" customWidth="1"/>
     <col min="5" max="5" width="12.54296875" customWidth="1"/>
     <col min="6" max="6" width="15.26953125" customWidth="1"/>
-    <col min="7" max="7" width="24.36328125" customWidth="1"/>
+    <col min="7" max="7" width="24.36328125" style="12" customWidth="1"/>
     <col min="8" max="8" width="20.54296875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1350,7 +1387,7 @@
       <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="11" t="s">
         <v>6</v>
       </c>
       <c r="H1" s="2" t="s">
@@ -1374,7 +1411,7 @@
       <c r="F2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="G2" s="10" t="s">
         <v>16</v>
       </c>
       <c r="H2" s="1" t="s">
@@ -1399,7 +1436,7 @@
       <c r="F3" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="G3" s="10" t="s">
         <v>16</v>
       </c>
       <c r="H3" s="1" t="s">
@@ -1407,7 +1444,7 @@
       </c>
       <c r="I3" s="1"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>18</v>
       </c>
@@ -1424,7 +1461,7 @@
       <c r="F4" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="G4" s="10" t="s">
         <v>22</v>
       </c>
       <c r="H4" s="1" t="s">
@@ -1445,7 +1482,7 @@
       <c r="E5">
         <v>202348</v>
       </c>
-      <c r="G5" s="1"/>
+      <c r="G5" s="10"/>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
     </row>
@@ -1459,7 +1496,7 @@
       <c r="E6">
         <v>116032</v>
       </c>
-      <c r="G6" s="1"/>
+      <c r="G6" s="10"/>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
     </row>
@@ -1476,7 +1513,7 @@
       <c r="E7">
         <v>114140</v>
       </c>
-      <c r="G7" s="1"/>
+      <c r="G7" s="10"/>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
     </row>
@@ -1497,7 +1534,7 @@
       <c r="F8" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="G8" s="1" t="s">
+      <c r="G8" s="10" t="s">
         <v>16</v>
       </c>
       <c r="H8" s="1" t="s">
@@ -1518,7 +1555,7 @@
       <c r="E9">
         <v>98265</v>
       </c>
-      <c r="G9" s="1"/>
+      <c r="G9" s="10"/>
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
     </row>
@@ -1560,7 +1597,7 @@
       <c r="F11" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="G11" s="1" t="s">
+      <c r="G11" s="10" t="s">
         <v>16</v>
       </c>
       <c r="H11" s="1" t="s">
@@ -1585,7 +1622,7 @@
       <c r="F12" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="G12" s="1" t="s">
+      <c r="G12" s="10" t="s">
         <v>16</v>
       </c>
       <c r="H12" s="1" t="s">
@@ -1608,7 +1645,7 @@
         <v>89598</v>
       </c>
       <c r="F13" s="1"/>
-      <c r="G13" s="1"/>
+      <c r="G13" s="10"/>
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
     </row>
@@ -1627,11 +1664,11 @@
         <v>88733</v>
       </c>
       <c r="F14" s="1"/>
-      <c r="G14" s="1"/>
+      <c r="G14" s="10"/>
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>54</v>
       </c>
@@ -1647,7 +1684,7 @@
       <c r="F15" t="s">
         <v>11</v>
       </c>
-      <c r="G15" s="1" t="s">
+      <c r="G15" s="10" t="s">
         <v>290</v>
       </c>
       <c r="H15" s="1" t="s">
@@ -1674,7 +1711,7 @@
       <c r="F16" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="G16" s="1" t="s">
+      <c r="G16" s="10" t="s">
         <v>291</v>
       </c>
       <c r="H16" s="1" t="s">
@@ -1699,7 +1736,7 @@
       <c r="F17" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="G17" s="1" t="s">
+      <c r="G17" s="10" t="s">
         <v>293</v>
       </c>
       <c r="H17" s="1" t="s">
@@ -1707,7 +1744,7 @@
       </c>
       <c r="I17" s="1"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>63</v>
       </c>
@@ -1724,7 +1761,7 @@
       <c r="F18" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="G18" s="1" t="s">
+      <c r="G18" s="10" t="s">
         <v>298</v>
       </c>
       <c r="H18" s="1" t="s">
@@ -1747,7 +1784,7 @@
         <v>74650</v>
       </c>
       <c r="F19" s="1"/>
-      <c r="G19" s="1"/>
+      <c r="G19" s="10"/>
       <c r="H19" s="1" t="s">
         <v>295</v>
       </c>
@@ -1769,7 +1806,7 @@
       <c r="F20" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="G20" s="1" t="s">
+      <c r="G20" s="10" t="s">
         <v>16</v>
       </c>
       <c r="H20" s="1" t="s">
@@ -1793,7 +1830,7 @@
       <c r="F21" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="G21" s="1" t="s">
+      <c r="G21" s="10" t="s">
         <v>16</v>
       </c>
       <c r="H21" s="1" t="s">
@@ -1816,7 +1853,7 @@
         <v>65257</v>
       </c>
       <c r="F22" s="1"/>
-      <c r="G22" s="1"/>
+      <c r="G22" s="10"/>
       <c r="H22" s="1"/>
       <c r="I22" s="1"/>
     </row>
@@ -1837,7 +1874,7 @@
       <c r="F23" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="G23" s="1" t="s">
+      <c r="G23" s="10" t="s">
         <v>16</v>
       </c>
       <c r="H23" s="1" t="s">
@@ -1862,7 +1899,7 @@
       <c r="F24" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="G24" s="1" t="s">
+      <c r="G24" s="10" t="s">
         <v>16</v>
       </c>
       <c r="H24" s="1" t="s">
@@ -1885,7 +1922,7 @@
         <v>61158</v>
       </c>
       <c r="F25" s="1"/>
-      <c r="G25" s="1"/>
+      <c r="G25" s="10"/>
       <c r="H25" s="1"/>
       <c r="I25" s="1"/>
     </row>
@@ -1905,7 +1942,7 @@
       <c r="F26" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="G26" s="1" t="s">
+      <c r="G26" s="10" t="s">
         <v>16</v>
       </c>
       <c r="H26" s="1" t="s">
@@ -1913,7 +1950,7 @@
       </c>
       <c r="I26" s="1"/>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:9" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>86</v>
       </c>
@@ -1929,9 +1966,15 @@
       <c r="E27">
         <v>60140</v>
       </c>
-      <c r="F27" s="1"/>
-      <c r="G27" s="1"/>
-      <c r="H27" s="1"/>
+      <c r="F27" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G27" s="10" t="s">
+        <v>300</v>
+      </c>
+      <c r="H27" s="1" t="s">
+        <v>299</v>
+      </c>
       <c r="I27" s="1"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.35">
@@ -1949,7 +1992,7 @@
         <v>59089</v>
       </c>
       <c r="F28" s="1"/>
-      <c r="G28" s="1"/>
+      <c r="G28" s="10"/>
       <c r="H28" s="1"/>
       <c r="I28" s="1"/>
     </row>
@@ -1966,7 +2009,7 @@
       <c r="E29">
         <v>58698</v>
       </c>
-      <c r="G29" s="1"/>
+      <c r="G29" s="10"/>
       <c r="H29" s="1"/>
       <c r="I29" s="1"/>
     </row>
@@ -1985,7 +2028,7 @@
         <v>58418</v>
       </c>
       <c r="F30" s="1"/>
-      <c r="G30" s="1"/>
+      <c r="G30" s="10"/>
       <c r="H30" s="1"/>
       <c r="I30" s="1"/>
     </row>
@@ -2004,7 +2047,7 @@
         <v>57005</v>
       </c>
       <c r="F31" s="1"/>
-      <c r="G31" s="1"/>
+      <c r="G31" s="10"/>
       <c r="H31" s="1"/>
       <c r="I31" s="1"/>
     </row>
@@ -2023,7 +2066,7 @@
         <v>55989</v>
       </c>
       <c r="F32" s="1"/>
-      <c r="G32" s="1"/>
+      <c r="G32" s="10"/>
       <c r="H32" s="1"/>
       <c r="I32" s="1"/>
     </row>
@@ -2037,7 +2080,7 @@
       <c r="E33">
         <v>55963</v>
       </c>
-      <c r="G33" s="1"/>
+      <c r="G33" s="10"/>
       <c r="H33" s="1"/>
       <c r="I33" s="1"/>
     </row>
@@ -2056,7 +2099,7 @@
         <v>55472</v>
       </c>
       <c r="F34" s="1"/>
-      <c r="G34" s="1"/>
+      <c r="G34" s="10"/>
       <c r="H34" s="1"/>
       <c r="I34" s="1"/>
     </row>
@@ -2077,7 +2120,7 @@
         <v>53282</v>
       </c>
       <c r="F35" s="1"/>
-      <c r="G35" s="1"/>
+      <c r="G35" s="10"/>
       <c r="H35" s="1"/>
       <c r="I35" s="1"/>
     </row>
@@ -2096,7 +2139,7 @@
         <v>51536</v>
       </c>
       <c r="F36" s="1"/>
-      <c r="G36" s="1"/>
+      <c r="G36" s="10"/>
       <c r="H36" s="1"/>
       <c r="I36" s="1"/>
     </row>
@@ -2115,7 +2158,7 @@
         <v>51326</v>
       </c>
       <c r="F37" s="1"/>
-      <c r="G37" s="1"/>
+      <c r="G37" s="10"/>
       <c r="H37" s="1"/>
       <c r="I37" s="1"/>
     </row>
@@ -2136,7 +2179,7 @@
         <v>50650</v>
       </c>
       <c r="F38" s="1"/>
-      <c r="G38" s="1"/>
+      <c r="G38" s="10"/>
       <c r="H38" s="1"/>
       <c r="I38" s="1"/>
     </row>
@@ -2155,7 +2198,7 @@
         <v>50596</v>
       </c>
       <c r="F39" s="1"/>
-      <c r="G39" s="1"/>
+      <c r="G39" s="10"/>
       <c r="H39" s="1"/>
       <c r="I39" s="1"/>
     </row>
@@ -2176,7 +2219,7 @@
         <v>50301</v>
       </c>
       <c r="F40" s="1"/>
-      <c r="G40" s="1"/>
+      <c r="G40" s="10"/>
       <c r="H40" s="1"/>
       <c r="I40" s="1"/>
     </row>
@@ -2193,7 +2236,7 @@
       <c r="E41">
         <v>49974</v>
       </c>
-      <c r="G41" s="1"/>
+      <c r="G41" s="10"/>
       <c r="H41" s="1"/>
       <c r="I41" s="1"/>
     </row>
@@ -2212,7 +2255,7 @@
         <v>48982</v>
       </c>
       <c r="F42" s="1"/>
-      <c r="G42" s="1"/>
+      <c r="G42" s="10"/>
       <c r="H42" s="1"/>
       <c r="I42" s="1"/>
     </row>
@@ -2231,7 +2274,7 @@
         <v>48295</v>
       </c>
       <c r="F43" s="1"/>
-      <c r="G43" s="1"/>
+      <c r="G43" s="10"/>
       <c r="H43" s="1"/>
       <c r="I43" s="1"/>
     </row>
@@ -2248,7 +2291,7 @@
       <c r="E44">
         <v>48271</v>
       </c>
-      <c r="G44" s="1"/>
+      <c r="G44" s="10"/>
       <c r="H44" s="1"/>
       <c r="I44" s="1"/>
     </row>
@@ -2267,7 +2310,7 @@
         <v>46616</v>
       </c>
       <c r="F45" s="1"/>
-      <c r="G45" s="1"/>
+      <c r="G45" s="10"/>
       <c r="H45" s="1"/>
       <c r="I45" s="1"/>
     </row>
@@ -2288,7 +2331,7 @@
       <c r="F46" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="G46" s="1" t="s">
+      <c r="G46" s="10" t="s">
         <v>284</v>
       </c>
       <c r="H46" s="1"/>
@@ -2310,7 +2353,7 @@
       <c r="E47">
         <v>46087</v>
       </c>
-      <c r="G47" s="1"/>
+      <c r="G47" s="10"/>
       <c r="H47" s="1"/>
       <c r="I47" s="1"/>
     </row>
@@ -2327,7 +2370,7 @@
       <c r="E48">
         <v>45189</v>
       </c>
-      <c r="G48" s="1"/>
+      <c r="G48" s="10"/>
       <c r="H48" s="1"/>
       <c r="I48" s="1"/>
     </row>
@@ -2348,7 +2391,7 @@
         <v>43716</v>
       </c>
       <c r="F49" s="1"/>
-      <c r="G49" s="1"/>
+      <c r="G49" s="10"/>
       <c r="H49" s="1"/>
       <c r="I49" s="1"/>
     </row>
@@ -2367,7 +2410,7 @@
         <v>43063</v>
       </c>
       <c r="F50" s="1"/>
-      <c r="G50" s="1"/>
+      <c r="G50" s="10"/>
       <c r="H50" s="1"/>
       <c r="I50" s="1"/>
     </row>
@@ -2386,7 +2429,7 @@
         <v>43000</v>
       </c>
       <c r="F51" s="1"/>
-      <c r="G51" s="1"/>
+      <c r="G51" s="10"/>
       <c r="H51" s="1"/>
       <c r="I51" s="1"/>
     </row>
@@ -2405,7 +2448,7 @@
         <v>42844</v>
       </c>
       <c r="F52" s="1"/>
-      <c r="G52" s="1"/>
+      <c r="G52" s="10"/>
       <c r="H52" s="1"/>
       <c r="I52" s="1"/>
     </row>
@@ -2426,7 +2469,7 @@
       <c r="F53" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="G53" s="9" t="s">
+      <c r="G53" s="13" t="s">
         <v>284</v>
       </c>
       <c r="H53" s="1"/>
@@ -2447,7 +2490,7 @@
         <v>42125</v>
       </c>
       <c r="F54" s="1"/>
-      <c r="G54" s="1"/>
+      <c r="G54" s="10"/>
       <c r="H54" s="1"/>
       <c r="I54" s="1"/>
     </row>
@@ -2466,7 +2509,7 @@
         <v>41982</v>
       </c>
       <c r="F55" s="1"/>
-      <c r="G55" s="1"/>
+      <c r="G55" s="10"/>
       <c r="H55" s="1"/>
       <c r="I55" s="1"/>
     </row>
@@ -2485,7 +2528,7 @@
         <v>41328</v>
       </c>
       <c r="F56" s="1"/>
-      <c r="G56" s="1"/>
+      <c r="G56" s="10"/>
       <c r="H56" s="1"/>
       <c r="I56" s="1"/>
     </row>
@@ -2505,7 +2548,7 @@
       <c r="E57">
         <v>41217</v>
       </c>
-      <c r="G57" s="1"/>
+      <c r="G57" s="10"/>
       <c r="H57" s="1"/>
       <c r="I57" s="1"/>
     </row>
@@ -2524,7 +2567,7 @@
         <v>41191</v>
       </c>
       <c r="F58" s="1"/>
-      <c r="G58" s="1"/>
+      <c r="G58" s="10"/>
       <c r="H58" s="1"/>
       <c r="I58" s="1"/>
     </row>
@@ -2545,7 +2588,7 @@
         <v>40911</v>
       </c>
       <c r="F59" s="1"/>
-      <c r="G59" s="1"/>
+      <c r="G59" s="10"/>
       <c r="H59" s="1"/>
       <c r="I59" s="1"/>
     </row>
@@ -2564,7 +2607,7 @@
         <v>40779</v>
       </c>
       <c r="F60" s="1"/>
-      <c r="G60" s="1"/>
+      <c r="G60" s="10"/>
       <c r="H60" s="1"/>
       <c r="I60" s="1"/>
     </row>
@@ -2583,7 +2626,7 @@
         <v>39632</v>
       </c>
       <c r="F61" s="1"/>
-      <c r="G61" s="1"/>
+      <c r="G61" s="10"/>
       <c r="H61" s="1"/>
       <c r="I61" s="1"/>
     </row>
@@ -2602,7 +2645,7 @@
         <v>39343</v>
       </c>
       <c r="F62" s="1"/>
-      <c r="G62" s="1"/>
+      <c r="G62" s="10"/>
       <c r="H62" s="1"/>
       <c r="I62" s="1"/>
     </row>
@@ -2623,7 +2666,7 @@
         <v>38638</v>
       </c>
       <c r="F63" s="1"/>
-      <c r="G63" s="1"/>
+      <c r="G63" s="10"/>
       <c r="H63" s="1"/>
       <c r="I63" s="1"/>
     </row>
@@ -2642,7 +2685,7 @@
         <v>38210</v>
       </c>
       <c r="F64" s="1"/>
-      <c r="G64" s="1"/>
+      <c r="G64" s="10"/>
       <c r="H64" s="1"/>
       <c r="I64" s="1"/>
     </row>
@@ -2662,7 +2705,7 @@
       <c r="E65">
         <v>38197</v>
       </c>
-      <c r="G65" s="1"/>
+      <c r="G65" s="10"/>
       <c r="H65" s="1"/>
       <c r="I65" s="1"/>
     </row>
@@ -2681,7 +2724,7 @@
         <v>37777</v>
       </c>
       <c r="F66" s="1"/>
-      <c r="G66" s="1"/>
+      <c r="G66" s="10"/>
       <c r="H66" s="1"/>
       <c r="I66" s="1"/>
     </row>
@@ -2700,7 +2743,7 @@
         <v>37277</v>
       </c>
       <c r="F67" s="1"/>
-      <c r="G67" s="1"/>
+      <c r="G67" s="10"/>
       <c r="H67" s="1"/>
       <c r="I67" s="1"/>
     </row>
@@ -2719,7 +2762,7 @@
         <v>36289</v>
       </c>
       <c r="F68" s="1"/>
-      <c r="G68" s="1"/>
+      <c r="G68" s="10"/>
       <c r="H68" s="1"/>
       <c r="I68" s="1"/>
     </row>
@@ -2736,7 +2779,7 @@
       <c r="E69">
         <v>36139</v>
       </c>
-      <c r="G69" s="1"/>
+      <c r="G69" s="10"/>
       <c r="H69" s="1"/>
       <c r="I69" s="1"/>
     </row>
@@ -2755,7 +2798,7 @@
         <v>35538</v>
       </c>
       <c r="F70" s="1"/>
-      <c r="G70" s="1"/>
+      <c r="G70" s="10"/>
       <c r="H70" s="1"/>
       <c r="I70" s="1"/>
     </row>
@@ -2774,7 +2817,7 @@
         <v>34473</v>
       </c>
       <c r="F71" s="1"/>
-      <c r="G71" s="1"/>
+      <c r="G71" s="10"/>
       <c r="H71" s="1"/>
       <c r="I71" s="1"/>
     </row>
@@ -2795,7 +2838,7 @@
       <c r="F72" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="G72" s="1" t="s">
+      <c r="G72" s="10" t="s">
         <v>284</v>
       </c>
       <c r="H72" s="1"/>
@@ -2816,7 +2859,7 @@
         <v>32032</v>
       </c>
       <c r="F73" s="1"/>
-      <c r="G73" s="1"/>
+      <c r="G73" s="10"/>
       <c r="H73" s="1"/>
       <c r="I73" s="1"/>
     </row>
@@ -2835,7 +2878,7 @@
         <v>31168</v>
       </c>
       <c r="F74" s="1"/>
-      <c r="G74" s="1"/>
+      <c r="G74" s="10"/>
       <c r="H74" s="1"/>
       <c r="I74" s="1"/>
     </row>
@@ -2855,7 +2898,7 @@
       <c r="E75">
         <v>29827</v>
       </c>
-      <c r="G75" s="1"/>
+      <c r="G75" s="10"/>
       <c r="H75" s="1"/>
       <c r="I75" s="1"/>
     </row>
@@ -2876,7 +2919,7 @@
       <c r="F76" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="G76" s="1" t="s">
+      <c r="G76" s="10" t="s">
         <v>284</v>
       </c>
       <c r="H76" s="9"/>
@@ -2899,7 +2942,7 @@
         <v>29516</v>
       </c>
       <c r="F77" s="1"/>
-      <c r="G77" s="1"/>
+      <c r="G77" s="10"/>
       <c r="H77" s="1"/>
       <c r="I77" s="1"/>
     </row>
@@ -2915,7 +2958,7 @@
         <v>28572</v>
       </c>
       <c r="F78" s="1"/>
-      <c r="G78" s="1"/>
+      <c r="G78" s="10"/>
       <c r="H78" s="1"/>
       <c r="I78" s="1"/>
     </row>
@@ -2936,7 +2979,7 @@
         <v>27743</v>
       </c>
       <c r="F79" s="1"/>
-      <c r="G79" s="1"/>
+      <c r="G79" s="10"/>
       <c r="H79" s="1"/>
       <c r="I79" s="1"/>
     </row>
@@ -2955,7 +2998,7 @@
         <v>27544</v>
       </c>
       <c r="F80" s="1"/>
-      <c r="G80" s="1"/>
+      <c r="G80" s="10"/>
       <c r="H80" s="1"/>
       <c r="I80" s="1"/>
     </row>
@@ -2974,7 +3017,7 @@
         <v>26482</v>
       </c>
       <c r="F81" s="1"/>
-      <c r="G81" s="1"/>
+      <c r="G81" s="10"/>
       <c r="H81" s="1"/>
       <c r="I81" s="1"/>
     </row>
@@ -2993,7 +3036,7 @@
         <v>25235</v>
       </c>
       <c r="F82" s="1"/>
-      <c r="G82" s="1"/>
+      <c r="G82" s="10"/>
       <c r="H82" s="1"/>
       <c r="I82" s="1"/>
     </row>
@@ -3010,7 +3053,7 @@
       <c r="E83">
         <v>25028</v>
       </c>
-      <c r="G83" s="1"/>
+      <c r="G83" s="10"/>
       <c r="H83" s="1"/>
       <c r="I83" s="1"/>
     </row>
@@ -3029,7 +3072,7 @@
         <v>23756</v>
       </c>
       <c r="F84" s="1"/>
-      <c r="G84" s="1"/>
+      <c r="G84" s="10"/>
       <c r="H84" s="1"/>
       <c r="I84" s="1"/>
     </row>
@@ -3049,7 +3092,7 @@
       <c r="E85">
         <v>22988</v>
       </c>
-      <c r="G85" s="1"/>
+      <c r="G85" s="10"/>
       <c r="H85" s="1"/>
       <c r="I85" s="1"/>
     </row>
@@ -3068,7 +3111,7 @@
         <v>22727</v>
       </c>
       <c r="F86" s="1"/>
-      <c r="G86" s="1"/>
+      <c r="G86" s="10"/>
       <c r="H86" s="1"/>
       <c r="I86" s="1"/>
     </row>
@@ -3087,7 +3130,7 @@
         <v>22663</v>
       </c>
       <c r="F87" s="1"/>
-      <c r="G87" s="1"/>
+      <c r="G87" s="10"/>
       <c r="H87" s="1"/>
       <c r="I87" s="1"/>
     </row>
@@ -3106,7 +3149,7 @@
         <v>22626</v>
       </c>
       <c r="F88" s="1"/>
-      <c r="G88" s="1"/>
+      <c r="G88" s="10"/>
       <c r="H88" s="1"/>
       <c r="I88" s="1"/>
     </row>
@@ -3125,7 +3168,7 @@
         <v>22518</v>
       </c>
       <c r="F89" s="1"/>
-      <c r="G89" s="1"/>
+      <c r="G89" s="10"/>
       <c r="H89" s="1"/>
       <c r="I89" s="1"/>
     </row>
@@ -3144,7 +3187,7 @@
         <v>21270</v>
       </c>
       <c r="F90" s="1"/>
-      <c r="G90" s="1"/>
+      <c r="G90" s="10"/>
       <c r="H90" s="1"/>
       <c r="I90" s="1"/>
     </row>
@@ -3161,7 +3204,7 @@
       <c r="E91">
         <v>20514</v>
       </c>
-      <c r="G91" s="1"/>
+      <c r="G91" s="10"/>
       <c r="H91" s="1"/>
       <c r="I91" s="1"/>
     </row>
@@ -3178,7 +3221,7 @@
       <c r="E92">
         <v>20133</v>
       </c>
-      <c r="G92" s="1"/>
+      <c r="G92" s="10"/>
       <c r="H92" s="1"/>
       <c r="I92" s="1"/>
     </row>
@@ -3197,7 +3240,7 @@
         <v>16280</v>
       </c>
       <c r="F93" s="1"/>
-      <c r="G93" s="1"/>
+      <c r="G93" s="10"/>
       <c r="H93" s="1"/>
       <c r="I93" s="1"/>
     </row>
@@ -3214,7 +3257,7 @@
       <c r="E94">
         <v>14272</v>
       </c>
-      <c r="G94" s="1"/>
+      <c r="G94" s="10"/>
       <c r="H94" s="1"/>
       <c r="I94" s="1"/>
     </row>
@@ -3233,7 +3276,7 @@
         <v>12641</v>
       </c>
       <c r="F95" s="1"/>
-      <c r="G95" s="1"/>
+      <c r="G95" s="10"/>
       <c r="H95" s="1"/>
       <c r="I95" s="1"/>
     </row>
@@ -3250,7 +3293,7 @@
       <c r="E96">
         <v>6178</v>
       </c>
-      <c r="G96" s="1"/>
+      <c r="G96" s="10"/>
       <c r="H96" s="1"/>
       <c r="I96" s="1"/>
     </row>
@@ -3271,7 +3314,7 @@
       <c r="F97" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="G97" s="1" t="s">
+      <c r="G97" s="10" t="s">
         <v>284</v>
       </c>
       <c r="H97" s="8"/>
@@ -3293,7 +3336,7 @@
       <c r="F98" t="s">
         <v>11</v>
       </c>
-      <c r="G98" t="s">
+      <c r="G98" s="12" t="s">
         <v>284</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Finished scraper for Abbenraa
</commit_message>
<xml_diff>
--- a/Kommuner.xlsx
+++ b/Kommuner.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\musse\OneDrive\UNI\9. semester\GitHub\First_Repository_CROW_FAR\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="62" documentId="11_FDF7A8DB94275223C5388096340570E2CE8365A4" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{3AC6DC05-7FC6-4537-815E-C5EC3501884E}"/>
+  <xr:revisionPtr revIDLastSave="65" documentId="11_FDF7A8DB94275223C5388096340570E2CE8365A4" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{EB3DE36D-F43E-44A9-BC6D-910A094CFC4D}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="301">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="380" uniqueCount="301">
   <si>
     <t>Kommuner</t>
   </si>
@@ -1354,7 +1354,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A27" sqref="A27"/>
+      <selection pane="bottomLeft" activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1991,9 +1991,15 @@
       <c r="E28">
         <v>59089</v>
       </c>
-      <c r="F28" s="1"/>
-      <c r="G28" s="10"/>
-      <c r="H28" s="1"/>
+      <c r="F28" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G28" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="H28" s="1" t="s">
+        <v>286</v>
+      </c>
       <c r="I28" s="1"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Created scraper for Hillerød
</commit_message>
<xml_diff>
--- a/Kommuner.xlsx
+++ b/Kommuner.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\musse\OneDrive\UNI\9. semester\GitHub\First_Repository_CROW_FAR\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="81" documentId="11_FDF7A8DB94275223C5388096340570E2CE8365A4" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{D75C63BA-E4D3-4734-9BE5-0408A2AAD404}"/>
+  <xr:revisionPtr revIDLastSave="86" documentId="11_FDF7A8DB94275223C5388096340570E2CE8365A4" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{030F6716-A993-429F-AE6C-273529B5A7DC}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="389" uniqueCount="303">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="304">
   <si>
     <t>Kommuner</t>
   </si>
@@ -946,6 +946,9 @@
   </si>
   <si>
     <t>2008 - 2017</t>
+  </si>
+  <si>
+    <t>JAVA</t>
   </si>
 </sst>
 </file>
@@ -1359,8 +1362,8 @@
   <dimension ref="A1:I99"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E36" sqref="E36"/>
+      <pane ySplit="1" topLeftCell="A34" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E39" sqref="E39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2179,7 +2182,7 @@
         <v>112</v>
       </c>
       <c r="B37" t="s">
-        <v>113</v>
+        <v>303</v>
       </c>
       <c r="C37" s="6" t="s">
         <v>114</v>
@@ -2209,9 +2212,15 @@
       <c r="E38">
         <v>50650</v>
       </c>
-      <c r="F38" s="1"/>
-      <c r="G38" s="10"/>
-      <c r="H38" s="1"/>
+      <c r="F38" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G38" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="H38" s="1" t="s">
+        <v>290</v>
+      </c>
       <c r="I38" s="1"/>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Created scraper for Greve, Kalundborg and Varde
</commit_message>
<xml_diff>
--- a/Kommuner.xlsx
+++ b/Kommuner.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\musse\OneDrive\UNI\9. semester\GitHub\First_Repository_CROW_FAR\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="86" documentId="11_FDF7A8DB94275223C5388096340570E2CE8365A4" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{030F6716-A993-429F-AE6C-273529B5A7DC}"/>
+  <xr:revisionPtr revIDLastSave="99" documentId="11_FDF7A8DB94275223C5388096340570E2CE8365A4" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{0E2CBF0C-3B67-49D1-A999-641AB7B777B1}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="304">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="400" uniqueCount="303">
   <si>
     <t>Kommuner</t>
   </si>
@@ -391,12 +391,6 @@
   </si>
   <si>
     <t>Varde</t>
-  </si>
-  <si>
-    <t>PDF - shitty polweb (Nothing before 2013)</t>
-  </si>
-  <si>
-    <t>https://preparepublic.vardekommune.dk/</t>
   </si>
   <si>
     <t>http://polweb.varde.dk/SitePages/Startside.aspx</t>
@@ -949,6 +943,9 @@
   </si>
   <si>
     <t>JAVA</t>
+  </si>
+  <si>
+    <t>Shitty polweb (Nothing before 2013)</t>
   </si>
 </sst>
 </file>
@@ -1362,8 +1359,8 @@
   <dimension ref="A1:I99"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A34" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E39" sqref="E39"/>
+      <pane ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G41" sqref="G41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1424,7 +1421,7 @@
         <v>16</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="I2" s="1"/>
     </row>
@@ -1547,7 +1544,7 @@
         <v>16</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="I8" s="1"/>
     </row>
@@ -1610,7 +1607,7 @@
         <v>16</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="I11" s="1"/>
     </row>
@@ -1635,7 +1632,7 @@
         <v>16</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="I12" s="1"/>
     </row>
@@ -1644,7 +1641,7 @@
         <v>49</v>
       </c>
       <c r="B13" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="C13" s="6" t="s">
         <v>51</v>
@@ -1663,7 +1660,7 @@
         <v>52</v>
       </c>
       <c r="B14" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="C14" s="6" t="s">
         <v>53</v>
@@ -1694,10 +1691,10 @@
         <v>11</v>
       </c>
       <c r="G15" s="10" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="I15" s="1"/>
     </row>
@@ -1706,7 +1703,7 @@
         <v>57</v>
       </c>
       <c r="B16" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="C16" s="6" t="s">
         <v>58</v>
@@ -1721,10 +1718,10 @@
         <v>11</v>
       </c>
       <c r="G16" s="10" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="I16" s="1"/>
     </row>
@@ -1746,10 +1743,10 @@
         <v>11</v>
       </c>
       <c r="G17" s="10" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="I17" s="1"/>
     </row>
@@ -1771,10 +1768,10 @@
         <v>11</v>
       </c>
       <c r="G18" s="10" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="I18" s="1"/>
     </row>
@@ -1783,7 +1780,7 @@
         <v>66</v>
       </c>
       <c r="B19" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="C19" s="6" t="s">
         <v>67</v>
@@ -1795,7 +1792,7 @@
       <c r="F19" s="1"/>
       <c r="G19" s="10"/>
       <c r="H19" s="1" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="I19" s="1"/>
     </row>
@@ -1819,7 +1816,7 @@
         <v>16</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="I20" s="1"/>
     </row>
@@ -1843,7 +1840,7 @@
         <v>16</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="I21" s="1"/>
     </row>
@@ -1887,7 +1884,7 @@
         <v>16</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="I23" s="1"/>
     </row>
@@ -1912,7 +1909,7 @@
         <v>16</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="I24" s="1"/>
     </row>
@@ -1921,7 +1918,7 @@
         <v>81</v>
       </c>
       <c r="B25" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="C25" s="6" t="s">
         <v>82</v>
@@ -1955,7 +1952,7 @@
         <v>16</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="I26" s="1"/>
     </row>
@@ -1979,10 +1976,10 @@
         <v>11</v>
       </c>
       <c r="G27" s="10" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="I27" s="1"/>
     </row>
@@ -2007,7 +2004,7 @@
         <v>16</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="I28" s="1"/>
     </row>
@@ -2016,7 +2013,7 @@
         <v>93</v>
       </c>
       <c r="B29" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="C29" s="6" t="s">
         <v>94</v>
@@ -2034,7 +2031,7 @@
         <v>95</v>
       </c>
       <c r="B30" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="C30" s="6" t="s">
         <v>96</v>
@@ -2072,7 +2069,7 @@
         <v>100</v>
       </c>
       <c r="B32" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="C32" s="6" t="s">
         <v>101</v>
@@ -2118,10 +2115,10 @@
         <v>11</v>
       </c>
       <c r="G34" s="10" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="H34" s="1" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="I34" s="1"/>
     </row>
@@ -2145,10 +2142,10 @@
         <v>11</v>
       </c>
       <c r="G35" s="10" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="H35" s="1" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="I35" s="1"/>
     </row>
@@ -2173,7 +2170,7 @@
         <v>16</v>
       </c>
       <c r="H36" s="1" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="I36" s="1"/>
     </row>
@@ -2182,7 +2179,7 @@
         <v>112</v>
       </c>
       <c r="B37" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="C37" s="6" t="s">
         <v>114</v>
@@ -2219,7 +2216,7 @@
         <v>16</v>
       </c>
       <c r="H38" s="1" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="I38" s="1"/>
     </row>
@@ -2247,67 +2244,83 @@
         <v>121</v>
       </c>
       <c r="B40" t="s">
+        <v>302</v>
+      </c>
+      <c r="C40" s="4" t="s">
         <v>122</v>
-      </c>
-      <c r="C40" s="6" t="s">
-        <v>123</v>
-      </c>
-      <c r="D40" s="4" t="s">
-        <v>124</v>
       </c>
       <c r="E40">
         <v>50301</v>
       </c>
-      <c r="F40" s="1"/>
-      <c r="G40" s="10"/>
-      <c r="H40" s="1"/>
+      <c r="F40" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G40" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="H40" s="1" t="s">
+        <v>293</v>
+      </c>
       <c r="I40" s="1"/>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B41" t="s">
         <v>61</v>
       </c>
       <c r="C41" s="6" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="E41">
         <v>49974</v>
       </c>
-      <c r="G41" s="10"/>
-      <c r="H41" s="1"/>
+      <c r="F41" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G41" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="H41" s="1" t="s">
+        <v>293</v>
+      </c>
       <c r="I41" s="1"/>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B42" t="s">
         <v>61</v>
       </c>
       <c r="C42" s="6" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="D42" s="1"/>
       <c r="E42">
         <v>48982</v>
       </c>
-      <c r="F42" s="1"/>
-      <c r="G42" s="10"/>
-      <c r="H42" s="1"/>
+      <c r="F42" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G42" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="H42" s="1" t="s">
+        <v>281</v>
+      </c>
       <c r="I42" s="1"/>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B43" t="s">
         <v>64</v>
       </c>
       <c r="C43" s="6" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="D43" s="1"/>
       <c r="E43">
@@ -2320,13 +2333,13 @@
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B44" t="s">
         <v>61</v>
       </c>
       <c r="C44" s="6" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="E44">
         <v>48271</v>
@@ -2337,13 +2350,13 @@
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
+        <v>131</v>
+      </c>
+      <c r="B45" t="s">
+        <v>132</v>
+      </c>
+      <c r="C45" s="6" t="s">
         <v>133</v>
-      </c>
-      <c r="B45" t="s">
-        <v>134</v>
-      </c>
-      <c r="C45" s="6" t="s">
-        <v>135</v>
       </c>
       <c r="D45" s="1"/>
       <c r="E45">
@@ -2356,13 +2369,13 @@
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B46" t="s">
         <v>61</v>
       </c>
       <c r="C46" s="6" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="D46" s="1"/>
       <c r="E46">
@@ -2372,23 +2385,23 @@
         <v>11</v>
       </c>
       <c r="G46" s="10" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="H46" s="1"/>
       <c r="I46" s="1"/>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
+        <v>136</v>
+      </c>
+      <c r="B47" t="s">
+        <v>137</v>
+      </c>
+      <c r="C47" s="6" t="s">
         <v>138</v>
       </c>
-      <c r="B47" t="s">
+      <c r="D47" s="6" t="s">
         <v>139</v>
-      </c>
-      <c r="C47" s="6" t="s">
-        <v>140</v>
-      </c>
-      <c r="D47" s="6" t="s">
-        <v>141</v>
       </c>
       <c r="E47">
         <v>46087</v>
@@ -2399,13 +2412,13 @@
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
+        <v>140</v>
+      </c>
+      <c r="B48" t="s">
+        <v>141</v>
+      </c>
+      <c r="C48" s="6" t="s">
         <v>142</v>
-      </c>
-      <c r="B48" t="s">
-        <v>143</v>
-      </c>
-      <c r="C48" s="6" t="s">
-        <v>144</v>
       </c>
       <c r="E48">
         <v>45189</v>
@@ -2416,16 +2429,16 @@
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B49" t="s">
         <v>55</v>
       </c>
       <c r="C49" s="6" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="D49" s="4" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="E49">
         <v>43716</v>
@@ -2437,13 +2450,13 @@
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
+        <v>146</v>
+      </c>
+      <c r="B50" s="7" t="s">
+        <v>147</v>
+      </c>
+      <c r="C50" s="6" t="s">
         <v>148</v>
-      </c>
-      <c r="B50" s="7" t="s">
-        <v>149</v>
-      </c>
-      <c r="C50" s="6" t="s">
-        <v>150</v>
       </c>
       <c r="D50" s="1"/>
       <c r="E50">
@@ -2456,13 +2469,13 @@
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B51" t="s">
         <v>55</v>
       </c>
       <c r="C51" s="6" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="D51" s="1"/>
       <c r="E51">
@@ -2475,13 +2488,13 @@
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B52" s="3" t="s">
         <v>74</v>
       </c>
       <c r="C52" s="6" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="D52" s="1"/>
       <c r="E52">
@@ -2494,13 +2507,13 @@
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B53" t="s">
         <v>64</v>
       </c>
       <c r="C53" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="D53" s="1"/>
       <c r="E53">
@@ -2510,20 +2523,20 @@
         <v>11</v>
       </c>
       <c r="G53" s="13" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="H53" s="1"/>
       <c r="I53" s="1"/>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B54" t="s">
         <v>19</v>
       </c>
       <c r="C54" s="6" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="D54" s="1"/>
       <c r="E54">
@@ -2536,13 +2549,13 @@
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
+        <v>157</v>
+      </c>
+      <c r="B55" t="s">
+        <v>158</v>
+      </c>
+      <c r="C55" s="6" t="s">
         <v>159</v>
-      </c>
-      <c r="B55" t="s">
-        <v>160</v>
-      </c>
-      <c r="C55" s="6" t="s">
-        <v>161</v>
       </c>
       <c r="D55" s="1"/>
       <c r="E55">
@@ -2555,13 +2568,13 @@
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
+        <v>160</v>
+      </c>
+      <c r="B56" t="s">
+        <v>161</v>
+      </c>
+      <c r="C56" s="6" t="s">
         <v>162</v>
-      </c>
-      <c r="B56" t="s">
-        <v>163</v>
-      </c>
-      <c r="C56" s="6" t="s">
-        <v>164</v>
       </c>
       <c r="D56" s="1"/>
       <c r="E56">
@@ -2574,16 +2587,16 @@
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B57" t="s">
         <v>33</v>
       </c>
       <c r="C57" s="6" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="D57" s="6" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="E57">
         <v>41217</v>
@@ -2594,13 +2607,13 @@
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
+        <v>166</v>
+      </c>
+      <c r="B58" t="s">
+        <v>167</v>
+      </c>
+      <c r="C58" s="6" t="s">
         <v>168</v>
-      </c>
-      <c r="B58" t="s">
-        <v>169</v>
-      </c>
-      <c r="C58" s="6" t="s">
-        <v>170</v>
       </c>
       <c r="D58" s="1"/>
       <c r="E58">
@@ -2613,16 +2626,16 @@
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
+        <v>169</v>
+      </c>
+      <c r="B59" t="s">
+        <v>170</v>
+      </c>
+      <c r="C59" s="6" t="s">
         <v>171</v>
       </c>
-      <c r="B59" t="s">
+      <c r="D59" s="6" t="s">
         <v>172</v>
-      </c>
-      <c r="C59" s="6" t="s">
-        <v>173</v>
-      </c>
-      <c r="D59" s="6" t="s">
-        <v>174</v>
       </c>
       <c r="E59">
         <v>40911</v>
@@ -2634,13 +2647,13 @@
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
+        <v>173</v>
+      </c>
+      <c r="B60" t="s">
+        <v>174</v>
+      </c>
+      <c r="C60" s="6" t="s">
         <v>175</v>
-      </c>
-      <c r="B60" t="s">
-        <v>176</v>
-      </c>
-      <c r="C60" s="6" t="s">
-        <v>177</v>
       </c>
       <c r="D60" s="1"/>
       <c r="E60">
@@ -2653,13 +2666,13 @@
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
+        <v>176</v>
+      </c>
+      <c r="B61" t="s">
+        <v>177</v>
+      </c>
+      <c r="C61" s="6" t="s">
         <v>178</v>
-      </c>
-      <c r="B61" t="s">
-        <v>179</v>
-      </c>
-      <c r="C61" s="6" t="s">
-        <v>180</v>
       </c>
       <c r="D61" s="1"/>
       <c r="E61">
@@ -2672,13 +2685,13 @@
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
+        <v>179</v>
+      </c>
+      <c r="B62" t="s">
+        <v>180</v>
+      </c>
+      <c r="C62" s="6" t="s">
         <v>181</v>
-      </c>
-      <c r="B62" t="s">
-        <v>182</v>
-      </c>
-      <c r="C62" s="6" t="s">
-        <v>183</v>
       </c>
       <c r="D62" s="1"/>
       <c r="E62">
@@ -2691,16 +2704,16 @@
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
+        <v>182</v>
+      </c>
+      <c r="B63" t="s">
+        <v>183</v>
+      </c>
+      <c r="C63" s="6" t="s">
         <v>184</v>
       </c>
-      <c r="B63" t="s">
+      <c r="D63" s="6" t="s">
         <v>185</v>
-      </c>
-      <c r="C63" s="6" t="s">
-        <v>186</v>
-      </c>
-      <c r="D63" s="6" t="s">
-        <v>187</v>
       </c>
       <c r="E63">
         <v>38638</v>
@@ -2712,13 +2725,13 @@
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
+        <v>186</v>
+      </c>
+      <c r="B64" t="s">
+        <v>187</v>
+      </c>
+      <c r="C64" s="6" t="s">
         <v>188</v>
-      </c>
-      <c r="B64" t="s">
-        <v>189</v>
-      </c>
-      <c r="C64" s="6" t="s">
-        <v>190</v>
       </c>
       <c r="D64" s="1"/>
       <c r="E64">
@@ -2731,16 +2744,16 @@
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
+        <v>189</v>
+      </c>
+      <c r="B65" t="s">
+        <v>190</v>
+      </c>
+      <c r="C65" s="6" t="s">
         <v>191</v>
       </c>
-      <c r="B65" t="s">
+      <c r="D65" s="6" t="s">
         <v>192</v>
-      </c>
-      <c r="C65" s="6" t="s">
-        <v>193</v>
-      </c>
-      <c r="D65" s="6" t="s">
-        <v>194</v>
       </c>
       <c r="E65">
         <v>38197</v>
@@ -2751,13 +2764,13 @@
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
+        <v>193</v>
+      </c>
+      <c r="B66" s="5" t="s">
+        <v>194</v>
+      </c>
+      <c r="C66" s="6" t="s">
         <v>195</v>
-      </c>
-      <c r="B66" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="C66" s="6" t="s">
-        <v>197</v>
       </c>
       <c r="D66" s="1"/>
       <c r="E66">
@@ -2770,13 +2783,13 @@
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
+        <v>196</v>
+      </c>
+      <c r="B67" t="s">
+        <v>197</v>
+      </c>
+      <c r="C67" s="6" t="s">
         <v>198</v>
-      </c>
-      <c r="B67" t="s">
-        <v>199</v>
-      </c>
-      <c r="C67" s="6" t="s">
-        <v>200</v>
       </c>
       <c r="D67" s="1"/>
       <c r="E67">
@@ -2789,13 +2802,13 @@
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="B68" t="s">
         <v>55</v>
       </c>
       <c r="C68" s="6" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="D68" s="1"/>
       <c r="E68">
@@ -2808,13 +2821,13 @@
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="B69" t="s">
         <v>113</v>
       </c>
       <c r="C69" s="6" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="E69">
         <v>36139</v>
@@ -2825,13 +2838,13 @@
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="B70" t="s">
         <v>61</v>
       </c>
       <c r="C70" s="6" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="D70" s="1"/>
       <c r="E70">
@@ -2844,13 +2857,13 @@
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="B71" t="s">
         <v>30</v>
       </c>
       <c r="C71" s="6" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="D71" s="1"/>
       <c r="E71">
@@ -2863,13 +2876,13 @@
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="B72" t="s">
         <v>61</v>
       </c>
       <c r="C72" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="D72" s="1"/>
       <c r="E72">
@@ -2879,20 +2892,20 @@
         <v>11</v>
       </c>
       <c r="G72" s="10" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="H72" s="1"/>
       <c r="I72" s="1"/>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
+        <v>209</v>
+      </c>
+      <c r="B73" t="s">
+        <v>210</v>
+      </c>
+      <c r="C73" s="6" t="s">
         <v>211</v>
-      </c>
-      <c r="B73" t="s">
-        <v>212</v>
-      </c>
-      <c r="C73" s="6" t="s">
-        <v>213</v>
       </c>
       <c r="D73" s="1"/>
       <c r="E73">
@@ -2905,13 +2918,13 @@
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="B74" t="s">
         <v>55</v>
       </c>
       <c r="C74" s="6" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="D74" s="1"/>
       <c r="E74">
@@ -2924,16 +2937,16 @@
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="B75" t="s">
         <v>30</v>
       </c>
       <c r="C75" s="6" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="D75" s="6" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="E75">
         <v>29827</v>
@@ -2944,13 +2957,13 @@
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="B76" t="s">
         <v>61</v>
       </c>
       <c r="C76" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="D76" s="1"/>
       <c r="E76">
@@ -2960,23 +2973,23 @@
         <v>11</v>
       </c>
       <c r="G76" s="10" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="H76" s="9"/>
       <c r="I76" s="1"/>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
+        <v>219</v>
+      </c>
+      <c r="B77" t="s">
+        <v>220</v>
+      </c>
+      <c r="C77" s="6" t="s">
         <v>221</v>
       </c>
-      <c r="B77" t="s">
+      <c r="D77" s="6" t="s">
         <v>222</v>
-      </c>
-      <c r="C77" s="6" t="s">
-        <v>223</v>
-      </c>
-      <c r="D77" s="6" t="s">
-        <v>224</v>
       </c>
       <c r="E77">
         <v>29516</v>
@@ -2988,10 +3001,10 @@
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="B78" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="D78" s="1"/>
       <c r="E78">
@@ -3004,16 +3017,16 @@
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="B79" t="s">
         <v>33</v>
       </c>
       <c r="C79" s="6" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="D79" s="6" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="E79">
         <v>27743</v>
@@ -3025,13 +3038,13 @@
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
+        <v>228</v>
+      </c>
+      <c r="B80" t="s">
+        <v>229</v>
+      </c>
+      <c r="C80" s="6" t="s">
         <v>230</v>
-      </c>
-      <c r="B80" t="s">
-        <v>231</v>
-      </c>
-      <c r="C80" s="6" t="s">
-        <v>232</v>
       </c>
       <c r="D80" s="1"/>
       <c r="E80">
@@ -3044,13 +3057,13 @@
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="B81" t="s">
         <v>19</v>
       </c>
       <c r="C81" s="6" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="D81" s="1"/>
       <c r="E81">
@@ -3063,13 +3076,13 @@
     </row>
     <row r="82" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
+        <v>233</v>
+      </c>
+      <c r="B82" s="3" t="s">
+        <v>234</v>
+      </c>
+      <c r="C82" s="6" t="s">
         <v>235</v>
-      </c>
-      <c r="B82" s="3" t="s">
-        <v>236</v>
-      </c>
-      <c r="C82" s="6" t="s">
-        <v>237</v>
       </c>
       <c r="D82" s="1"/>
       <c r="E82">
@@ -3082,13 +3095,13 @@
     </row>
     <row r="83" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
+        <v>236</v>
+      </c>
+      <c r="B83" t="s">
+        <v>237</v>
+      </c>
+      <c r="C83" s="6" t="s">
         <v>238</v>
-      </c>
-      <c r="B83" t="s">
-        <v>239</v>
-      </c>
-      <c r="C83" s="6" t="s">
-        <v>240</v>
       </c>
       <c r="E83">
         <v>25028</v>
@@ -3099,13 +3112,13 @@
     </row>
     <row r="84" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
+        <v>239</v>
+      </c>
+      <c r="B84" t="s">
+        <v>240</v>
+      </c>
+      <c r="C84" s="6" t="s">
         <v>241</v>
-      </c>
-      <c r="B84" t="s">
-        <v>242</v>
-      </c>
-      <c r="C84" s="6" t="s">
-        <v>243</v>
       </c>
       <c r="D84" s="1"/>
       <c r="E84">
@@ -3118,16 +3131,16 @@
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
+        <v>242</v>
+      </c>
+      <c r="B85" t="s">
+        <v>243</v>
+      </c>
+      <c r="C85" s="6" t="s">
         <v>244</v>
       </c>
-      <c r="B85" t="s">
+      <c r="D85" s="6" t="s">
         <v>245</v>
-      </c>
-      <c r="C85" s="6" t="s">
-        <v>246</v>
-      </c>
-      <c r="D85" s="6" t="s">
-        <v>247</v>
       </c>
       <c r="E85">
         <v>22988</v>
@@ -3138,13 +3151,13 @@
     </row>
     <row r="86" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
+        <v>246</v>
+      </c>
+      <c r="B86" t="s">
+        <v>247</v>
+      </c>
+      <c r="C86" s="6" t="s">
         <v>248</v>
-      </c>
-      <c r="B86" t="s">
-        <v>249</v>
-      </c>
-      <c r="C86" s="6" t="s">
-        <v>250</v>
       </c>
       <c r="D86" s="1"/>
       <c r="E86">
@@ -3157,13 +3170,13 @@
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="B87" t="s">
         <v>71</v>
       </c>
       <c r="C87" s="6" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="D87" s="1"/>
       <c r="E87">
@@ -3176,13 +3189,13 @@
     </row>
     <row r="88" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
+        <v>251</v>
+      </c>
+      <c r="B88" t="s">
+        <v>252</v>
+      </c>
+      <c r="C88" s="6" t="s">
         <v>253</v>
-      </c>
-      <c r="B88" t="s">
-        <v>254</v>
-      </c>
-      <c r="C88" s="6" t="s">
-        <v>255</v>
       </c>
       <c r="D88" s="1"/>
       <c r="E88">
@@ -3195,13 +3208,13 @@
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="B89" t="s">
         <v>55</v>
       </c>
       <c r="C89" s="6" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="D89" s="1"/>
       <c r="E89">
@@ -3214,13 +3227,13 @@
     </row>
     <row r="90" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
+        <v>256</v>
+      </c>
+      <c r="B90" t="s">
+        <v>257</v>
+      </c>
+      <c r="C90" s="6" t="s">
         <v>258</v>
-      </c>
-      <c r="B90" t="s">
-        <v>259</v>
-      </c>
-      <c r="C90" s="6" t="s">
-        <v>260</v>
       </c>
       <c r="D90" s="1"/>
       <c r="E90">
@@ -3233,13 +3246,13 @@
     </row>
     <row r="91" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="B91" t="s">
         <v>61</v>
       </c>
       <c r="C91" s="6" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="E91">
         <v>20514</v>
@@ -3250,13 +3263,13 @@
     </row>
     <row r="92" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
+        <v>261</v>
+      </c>
+      <c r="B92" t="s">
+        <v>262</v>
+      </c>
+      <c r="C92" s="6" t="s">
         <v>263</v>
-      </c>
-      <c r="B92" t="s">
-        <v>264</v>
-      </c>
-      <c r="C92" s="6" t="s">
-        <v>265</v>
       </c>
       <c r="E92">
         <v>20133</v>
@@ -3267,13 +3280,13 @@
     </row>
     <row r="93" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
+        <v>264</v>
+      </c>
+      <c r="B93" t="s">
+        <v>265</v>
+      </c>
+      <c r="C93" s="6" t="s">
         <v>266</v>
-      </c>
-      <c r="B93" t="s">
-        <v>267</v>
-      </c>
-      <c r="C93" s="6" t="s">
-        <v>268</v>
       </c>
       <c r="D93" s="1"/>
       <c r="E93">
@@ -3286,13 +3299,13 @@
     </row>
     <row r="94" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="B94" t="s">
         <v>91</v>
       </c>
       <c r="C94" s="6" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="E94">
         <v>14272</v>
@@ -3303,13 +3316,13 @@
     </row>
     <row r="95" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="B95" t="s">
         <v>55</v>
       </c>
       <c r="C95" s="6" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="D95" s="1"/>
       <c r="E95">
@@ -3322,13 +3335,13 @@
     </row>
     <row r="96" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="B96" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="C96" s="6" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="E96">
         <v>6178</v>
@@ -3339,13 +3352,13 @@
     </row>
     <row r="97" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="B97" t="s">
         <v>61</v>
       </c>
       <c r="C97" s="6" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="D97" s="1"/>
       <c r="E97">
@@ -3355,20 +3368,20 @@
         <v>11</v>
       </c>
       <c r="G97" s="10" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="H97" s="8"/>
       <c r="I97" s="1"/>
     </row>
     <row r="98" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B98" t="s">
         <v>61</v>
       </c>
       <c r="C98" s="6" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="E98">
         <v>3401</v>
@@ -3377,18 +3390,18 @@
         <v>11</v>
       </c>
       <c r="G98" s="12" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
     </row>
     <row r="99" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
+        <v>277</v>
+      </c>
+      <c r="B99" t="s">
+        <v>278</v>
+      </c>
+      <c r="C99" s="6" t="s">
         <v>279</v>
-      </c>
-      <c r="B99" t="s">
-        <v>280</v>
-      </c>
-      <c r="C99" s="6" t="s">
-        <v>281</v>
       </c>
       <c r="E99">
         <v>1807</v>
@@ -3496,20 +3509,19 @@
     <hyperlink ref="C66" r:id="rId95" xr:uid="{00000000-0004-0000-0000-000060000000}"/>
     <hyperlink ref="C2" r:id="rId96" display="https://www.kk.dk/dagsordener-og-referater?field_committee_type_tid%5B%5D=13957&amp;field_committee_type_tid%5B%5D=13960&amp;field_committee_type_tid%5B%5D=13959&amp;field_committee_type_tid%5B%5D=13958&amp;title=&amp;field_date_single_value%5Bvalue%5D%5Bdate%5D=01.01.2007&amp;field_date_single_value_1%5Bvalue%5D%5Bdate%5D=01.01.2018" xr:uid="{00000000-0004-0000-0000-000061000000}"/>
     <hyperlink ref="C93" r:id="rId97" display="https://www.vallensbaek.dk/kommunen/dagsordner-og-referater/dagsordner-og-referater?meetings_date_from%5Bvalue%5D%5Bmonth%5D=7&amp;meetings_date_from%5Bvalue%5D%5Byear%5D=2013&amp;meetings_to_date%5Bvalue%5D%5Bmonth%5D=7&amp;meetings_to_date%5Bvalue%5D%5Byear%5D=2019&amp;field_os2web_meetings_committee_tid=All" xr:uid="{00000000-0004-0000-0000-000062000000}"/>
-    <hyperlink ref="C40" r:id="rId98" xr:uid="{00000000-0004-0000-0000-000063000000}"/>
-    <hyperlink ref="D40" r:id="rId99" xr:uid="{00000000-0004-0000-0000-000064000000}"/>
-    <hyperlink ref="C52" r:id="rId100" xr:uid="{00000000-0004-0000-0000-000065000000}"/>
-    <hyperlink ref="C7" r:id="rId101" xr:uid="{00000000-0004-0000-0000-000066000000}"/>
-    <hyperlink ref="C67" r:id="rId102" xr:uid="{00000000-0004-0000-0000-000067000000}"/>
-    <hyperlink ref="C10" r:id="rId103" xr:uid="{00000000-0004-0000-0000-000068000000}"/>
-    <hyperlink ref="D10" r:id="rId104" xr:uid="{00000000-0004-0000-0000-000069000000}"/>
-    <hyperlink ref="C47" r:id="rId105" xr:uid="{00000000-0004-0000-0000-00006A000000}"/>
-    <hyperlink ref="D47" r:id="rId106" xr:uid="{00000000-0004-0000-0000-00006B000000}"/>
-    <hyperlink ref="C96" r:id="rId107" xr:uid="{00000000-0004-0000-0000-00006C000000}"/>
-    <hyperlink ref="C4" r:id="rId108" xr:uid="{00000000-0004-0000-0000-00006D000000}"/>
-    <hyperlink ref="C5" r:id="rId109" xr:uid="{00000000-0004-0000-0000-00006E000000}"/>
+    <hyperlink ref="C40" r:id="rId98" xr:uid="{00000000-0004-0000-0000-000064000000}"/>
+    <hyperlink ref="C52" r:id="rId99" xr:uid="{00000000-0004-0000-0000-000065000000}"/>
+    <hyperlink ref="C7" r:id="rId100" xr:uid="{00000000-0004-0000-0000-000066000000}"/>
+    <hyperlink ref="C67" r:id="rId101" xr:uid="{00000000-0004-0000-0000-000067000000}"/>
+    <hyperlink ref="C10" r:id="rId102" xr:uid="{00000000-0004-0000-0000-000068000000}"/>
+    <hyperlink ref="D10" r:id="rId103" xr:uid="{00000000-0004-0000-0000-000069000000}"/>
+    <hyperlink ref="C47" r:id="rId104" xr:uid="{00000000-0004-0000-0000-00006A000000}"/>
+    <hyperlink ref="D47" r:id="rId105" xr:uid="{00000000-0004-0000-0000-00006B000000}"/>
+    <hyperlink ref="C96" r:id="rId106" xr:uid="{00000000-0004-0000-0000-00006C000000}"/>
+    <hyperlink ref="C4" r:id="rId107" xr:uid="{00000000-0004-0000-0000-00006D000000}"/>
+    <hyperlink ref="C5" r:id="rId108" xr:uid="{00000000-0004-0000-0000-00006E000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId110"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId109"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Scrapers for Favrskov og Skive
</commit_message>
<xml_diff>
--- a/Kommuner.xlsx
+++ b/Kommuner.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\musse\OneDrive\UNI\9. semester\GitHub\First_Repository_CROW_FAR\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="99" documentId="11_FDF7A8DB94275223C5388096340570E2CE8365A4" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{0E2CBF0C-3B67-49D1-A999-641AB7B777B1}"/>
+  <xr:revisionPtr revIDLastSave="105" documentId="11_FDF7A8DB94275223C5388096340570E2CE8365A4" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{4BE6B8B2-DD4C-4A23-B214-0514BB4F0A01}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="400" uniqueCount="303">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="404" uniqueCount="303">
   <si>
     <t>Kommuner</t>
   </si>
@@ -1359,8 +1359,8 @@
   <dimension ref="A1:I99"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G41" sqref="G41"/>
+      <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A46" sqref="A46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2344,8 +2344,15 @@
       <c r="E44">
         <v>48271</v>
       </c>
-      <c r="G44" s="10"/>
-      <c r="H44" s="1"/>
+      <c r="F44" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G44" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="H44" s="1" t="s">
+        <v>281</v>
+      </c>
       <c r="I44" s="1"/>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.35">
@@ -2385,9 +2392,11 @@
         <v>11</v>
       </c>
       <c r="G46" s="10" t="s">
-        <v>280</v>
-      </c>
-      <c r="H46" s="1"/>
+        <v>16</v>
+      </c>
+      <c r="H46" s="1" t="s">
+        <v>292</v>
+      </c>
       <c r="I46" s="1"/>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Scraper for Ballerup done
</commit_message>
<xml_diff>
--- a/Kommuner.xlsx
+++ b/Kommuner.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\musse\OneDrive\UNI\9. semester\GitHub\First_Repository_CROW_FAR\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="105" documentId="11_FDF7A8DB94275223C5388096340570E2CE8365A4" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{4BE6B8B2-DD4C-4A23-B214-0514BB4F0A01}"/>
+  <xr:revisionPtr revIDLastSave="109" documentId="11_FDF7A8DB94275223C5388096340570E2CE8365A4" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{EBB7CD40-45AE-4797-B875-5253C11DC188}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="404" uniqueCount="303">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="407" uniqueCount="303">
   <si>
     <t>Kommuner</t>
   </si>
@@ -1359,8 +1359,8 @@
   <dimension ref="A1:I99"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A46" sqref="A46"/>
+      <pane ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H43" sqref="H43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2225,7 +2225,7 @@
         <v>119</v>
       </c>
       <c r="B39" t="s">
-        <v>19</v>
+        <v>301</v>
       </c>
       <c r="C39" s="6" t="s">
         <v>120</v>
@@ -2326,9 +2326,15 @@
       <c r="E43">
         <v>48295</v>
       </c>
-      <c r="F43" s="1"/>
-      <c r="G43" s="10"/>
-      <c r="H43" s="1"/>
+      <c r="F43" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G43" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="H43" s="1" t="s">
+        <v>293</v>
+      </c>
       <c r="I43" s="1"/>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Created scrapers for Frederikssund og Vordingborg
</commit_message>
<xml_diff>
--- a/Kommuner.xlsx
+++ b/Kommuner.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\musse\OneDrive\UNI\9. semester\GitHub\First_Repository_CROW_FAR\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="112" documentId="11_FDF7A8DB94275223C5388096340570E2CE8365A4" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{43CF53B2-568F-4981-A98E-F96291004683}"/>
+  <xr:revisionPtr revIDLastSave="118" documentId="11_FDF7A8DB94275223C5388096340570E2CE8365A4" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{2E74CA42-8A7A-4D9B-B432-55A4D8BCDF62}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="410" uniqueCount="303">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="416" uniqueCount="305">
   <si>
     <t>Kommuner</t>
   </si>
@@ -946,6 +946,12 @@
   </si>
   <si>
     <t>Shitty polweb (Nothing before 2013)</t>
+  </si>
+  <si>
+    <t>Done - two separate scrapers and final files</t>
+  </si>
+  <si>
+    <t>2007- 2017</t>
   </si>
 </sst>
 </file>
@@ -1360,7 +1366,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H46" sqref="H46"/>
+      <selection pane="bottomLeft" activeCell="F49" sqref="F49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2411,7 +2417,7 @@
       </c>
       <c r="I46" s="1"/>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>136</v>
       </c>
@@ -2427,8 +2433,15 @@
       <c r="E47">
         <v>46087</v>
       </c>
-      <c r="G47" s="10"/>
-      <c r="H47" s="1"/>
+      <c r="F47" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G47" s="10" t="s">
+        <v>303</v>
+      </c>
+      <c r="H47" s="1" t="s">
+        <v>281</v>
+      </c>
       <c r="I47" s="1"/>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.35">
@@ -2444,8 +2457,15 @@
       <c r="E48">
         <v>45189</v>
       </c>
-      <c r="G48" s="10"/>
-      <c r="H48" s="1"/>
+      <c r="F48" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G48" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="H48" s="1" t="s">
+        <v>304</v>
+      </c>
       <c r="I48" s="1"/>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Scraper for Egedal done
</commit_message>
<xml_diff>
--- a/Kommuner.xlsx
+++ b/Kommuner.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\musse\OneDrive\UNI\9. semester\GitHub\First_Repository_CROW_FAR\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="6_{94E8BF82-5DD1-4261-9586-168A515FB7A7}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{D7CF34ED-5439-4534-AA3F-A9B7CF9C46A2}"/>
+  <xr:revisionPtr revIDLastSave="7" documentId="6_{94E8BF82-5DD1-4261-9586-168A515FB7A7}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{DF2559B3-3EBD-43DB-9A1B-2427381B1794}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="420" uniqueCount="306">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="423" uniqueCount="306">
   <si>
     <t>Kommuner</t>
   </si>
@@ -1369,7 +1369,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H50" sqref="H50"/>
+      <selection pane="bottomLeft" activeCell="H52" sqref="H52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2532,9 +2532,15 @@
       <c r="E51">
         <v>43000</v>
       </c>
-      <c r="F51" s="1"/>
-      <c r="G51" s="10"/>
-      <c r="H51" s="1"/>
+      <c r="F51" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G51" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="H51" s="1" t="s">
+        <v>283</v>
+      </c>
       <c r="I51" s="1"/>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Scraper for Ikast-Brande done
</commit_message>
<xml_diff>
--- a/Kommuner.xlsx
+++ b/Kommuner.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\musse\OneDrive\UNI\9. semester\GitHub\First_Repository_CROW_FAR\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="9" documentId="6_{94E8BF82-5DD1-4261-9586-168A515FB7A7}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{C377036E-A7A4-4E2E-9C83-D3FB1B932A64}"/>
+  <xr:revisionPtr revIDLastSave="19" documentId="6_{94E8BF82-5DD1-4261-9586-168A515FB7A7}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{D8B79E29-2842-4FA7-8CE5-11A450AA0225}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="424" uniqueCount="307">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="427" uniqueCount="307">
   <si>
     <t>Kommuner</t>
   </si>
@@ -501,16 +501,10 @@
     <t>Lolland</t>
   </si>
   <si>
-    <t>PDF - flash maybe? (nothing before 2015. Who ever made this website is a madman!)</t>
-  </si>
-  <si>
     <t>https://www.lolland.dk/politik/dagsordener-og-referater</t>
   </si>
   <si>
     <t>Assens</t>
-  </si>
-  <si>
-    <t>Polweb w/PDF</t>
   </si>
   <si>
     <t>http://polweb.assens.dk/SitePages/Startside.aspx</t>
@@ -958,6 +952,12 @@
   </si>
   <si>
     <t>2011 - 2017</t>
+  </si>
+  <si>
+    <t>JAVA PDF - maybe? (nothing before 2015. Who ever made this website is a madman!)</t>
+  </si>
+  <si>
+    <t>java? Polweb w/PDF</t>
   </si>
 </sst>
 </file>
@@ -1030,7 +1030,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1053,6 +1053,7 @@
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
@@ -1371,8 +1372,8 @@
   <dimension ref="A1:I99"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H53" sqref="H53"/>
+      <pane ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F58" sqref="F58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1433,7 +1434,7 @@
         <v>16</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="I2" s="1"/>
     </row>
@@ -1556,7 +1557,7 @@
         <v>16</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="I8" s="1"/>
     </row>
@@ -1619,7 +1620,7 @@
         <v>16</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="I11" s="1"/>
     </row>
@@ -1644,7 +1645,7 @@
         <v>16</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="I12" s="1"/>
     </row>
@@ -1653,7 +1654,7 @@
         <v>49</v>
       </c>
       <c r="B13" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="C13" s="6" t="s">
         <v>51</v>
@@ -1672,7 +1673,7 @@
         <v>52</v>
       </c>
       <c r="B14" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="C14" s="6" t="s">
         <v>53</v>
@@ -1703,10 +1704,10 @@
         <v>11</v>
       </c>
       <c r="G15" s="10" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="I15" s="1"/>
     </row>
@@ -1715,7 +1716,7 @@
         <v>57</v>
       </c>
       <c r="B16" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="C16" s="6" t="s">
         <v>58</v>
@@ -1730,10 +1731,10 @@
         <v>11</v>
       </c>
       <c r="G16" s="10" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="I16" s="1"/>
     </row>
@@ -1755,10 +1756,10 @@
         <v>11</v>
       </c>
       <c r="G17" s="10" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="I17" s="1"/>
     </row>
@@ -1780,10 +1781,10 @@
         <v>11</v>
       </c>
       <c r="G18" s="10" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="I18" s="1"/>
     </row>
@@ -1792,7 +1793,7 @@
         <v>66</v>
       </c>
       <c r="B19" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="C19" s="6" t="s">
         <v>67</v>
@@ -1804,7 +1805,7 @@
       <c r="F19" s="1"/>
       <c r="G19" s="10"/>
       <c r="H19" s="1" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="I19" s="1"/>
     </row>
@@ -1828,7 +1829,7 @@
         <v>16</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="I20" s="1"/>
     </row>
@@ -1852,7 +1853,7 @@
         <v>16</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="I21" s="1"/>
     </row>
@@ -1896,7 +1897,7 @@
         <v>16</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="I23" s="1"/>
     </row>
@@ -1921,7 +1922,7 @@
         <v>16</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="I24" s="1"/>
     </row>
@@ -1930,7 +1931,7 @@
         <v>81</v>
       </c>
       <c r="B25" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="C25" s="6" t="s">
         <v>82</v>
@@ -1964,7 +1965,7 @@
         <v>16</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="I26" s="1"/>
     </row>
@@ -1988,10 +1989,10 @@
         <v>11</v>
       </c>
       <c r="G27" s="10" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="I27" s="1"/>
     </row>
@@ -2016,7 +2017,7 @@
         <v>16</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="I28" s="1"/>
     </row>
@@ -2025,7 +2026,7 @@
         <v>93</v>
       </c>
       <c r="B29" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="C29" s="6" t="s">
         <v>94</v>
@@ -2043,7 +2044,7 @@
         <v>95</v>
       </c>
       <c r="B30" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="C30" s="6" t="s">
         <v>96</v>
@@ -2081,7 +2082,7 @@
         <v>100</v>
       </c>
       <c r="B32" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="C32" s="6" t="s">
         <v>101</v>
@@ -2127,10 +2128,10 @@
         <v>11</v>
       </c>
       <c r="G34" s="10" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="H34" s="1" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="I34" s="1"/>
     </row>
@@ -2154,10 +2155,10 @@
         <v>11</v>
       </c>
       <c r="G35" s="10" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="H35" s="1" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="I35" s="1"/>
     </row>
@@ -2182,7 +2183,7 @@
         <v>16</v>
       </c>
       <c r="H36" s="1" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="I36" s="1"/>
     </row>
@@ -2191,7 +2192,7 @@
         <v>112</v>
       </c>
       <c r="B37" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="C37" s="6" t="s">
         <v>114</v>
@@ -2228,7 +2229,7 @@
         <v>16</v>
       </c>
       <c r="H38" s="1" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="I38" s="1"/>
     </row>
@@ -2237,7 +2238,7 @@
         <v>119</v>
       </c>
       <c r="B39" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="C39" s="6" t="s">
         <v>120</v>
@@ -2256,7 +2257,7 @@
         <v>121</v>
       </c>
       <c r="B40" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="C40" s="4" t="s">
         <v>122</v>
@@ -2271,7 +2272,7 @@
         <v>16</v>
       </c>
       <c r="H40" s="1" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="I40" s="1"/>
     </row>
@@ -2295,7 +2296,7 @@
         <v>16</v>
       </c>
       <c r="H41" s="1" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="I41" s="1"/>
     </row>
@@ -2320,7 +2321,7 @@
         <v>16</v>
       </c>
       <c r="H42" s="1" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="I42" s="1"/>
     </row>
@@ -2345,7 +2346,7 @@
         <v>16</v>
       </c>
       <c r="H43" s="1" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="I43" s="1"/>
     </row>
@@ -2369,7 +2370,7 @@
         <v>16</v>
       </c>
       <c r="H44" s="1" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="I44" s="1"/>
     </row>
@@ -2394,7 +2395,7 @@
         <v>16</v>
       </c>
       <c r="H45" s="1" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="I45" s="1"/>
     </row>
@@ -2419,7 +2420,7 @@
         <v>16</v>
       </c>
       <c r="H46" s="1" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="I46" s="1"/>
     </row>
@@ -2443,10 +2444,10 @@
         <v>11</v>
       </c>
       <c r="G47" s="10" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="H47" s="1" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="I47" s="1"/>
     </row>
@@ -2454,7 +2455,7 @@
       <c r="A48" t="s">
         <v>140</v>
       </c>
-      <c r="B48" t="s">
+      <c r="B48" s="14" t="s">
         <v>141</v>
       </c>
       <c r="C48" s="6" t="s">
@@ -2470,7 +2471,7 @@
         <v>16</v>
       </c>
       <c r="H48" s="1" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="I48" s="1"/>
     </row>
@@ -2492,7 +2493,7 @@
       </c>
       <c r="F49" s="1"/>
       <c r="H49" s="1" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="I49" s="1"/>
     </row>
@@ -2517,7 +2518,7 @@
         <v>16</v>
       </c>
       <c r="H50" s="1" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="I50" s="1"/>
     </row>
@@ -2542,7 +2543,7 @@
         <v>16</v>
       </c>
       <c r="H51" s="1" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="I51" s="1"/>
     </row>
@@ -2586,7 +2587,7 @@
         <v>16</v>
       </c>
       <c r="H53" s="1" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="I53" s="1"/>
     </row>
@@ -2595,7 +2596,7 @@
         <v>155</v>
       </c>
       <c r="B54" t="s">
-        <v>19</v>
+        <v>299</v>
       </c>
       <c r="C54" s="6" t="s">
         <v>156</v>
@@ -2614,10 +2615,10 @@
         <v>157</v>
       </c>
       <c r="B55" t="s">
+        <v>305</v>
+      </c>
+      <c r="C55" s="6" t="s">
         <v>158</v>
-      </c>
-      <c r="C55" s="6" t="s">
-        <v>159</v>
       </c>
       <c r="D55" s="1"/>
       <c r="E55">
@@ -2630,13 +2631,13 @@
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
+        <v>159</v>
+      </c>
+      <c r="B56" t="s">
+        <v>306</v>
+      </c>
+      <c r="C56" s="6" t="s">
         <v>160</v>
-      </c>
-      <c r="B56" t="s">
-        <v>161</v>
-      </c>
-      <c r="C56" s="6" t="s">
-        <v>162</v>
       </c>
       <c r="D56" s="1"/>
       <c r="E56">
@@ -2649,16 +2650,16 @@
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
+        <v>161</v>
+      </c>
+      <c r="B57" t="s">
+        <v>299</v>
+      </c>
+      <c r="C57" s="6" t="s">
+        <v>162</v>
+      </c>
+      <c r="D57" s="6" t="s">
         <v>163</v>
-      </c>
-      <c r="B57" t="s">
-        <v>33</v>
-      </c>
-      <c r="C57" s="6" t="s">
-        <v>164</v>
-      </c>
-      <c r="D57" s="6" t="s">
-        <v>165</v>
       </c>
       <c r="E57">
         <v>41217</v>
@@ -2669,35 +2670,41 @@
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
+        <v>164</v>
+      </c>
+      <c r="B58" t="s">
+        <v>165</v>
+      </c>
+      <c r="C58" s="6" t="s">
         <v>166</v>
-      </c>
-      <c r="B58" t="s">
-        <v>167</v>
-      </c>
-      <c r="C58" s="6" t="s">
-        <v>168</v>
       </c>
       <c r="D58" s="1"/>
       <c r="E58">
         <v>41191</v>
       </c>
-      <c r="F58" s="1"/>
-      <c r="G58" s="10"/>
-      <c r="H58" s="1"/>
+      <c r="F58" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G58" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="H58" s="1" t="s">
+        <v>286</v>
+      </c>
       <c r="I58" s="1"/>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
+        <v>167</v>
+      </c>
+      <c r="B59" t="s">
+        <v>168</v>
+      </c>
+      <c r="C59" s="6" t="s">
         <v>169</v>
       </c>
-      <c r="B59" t="s">
+      <c r="D59" s="6" t="s">
         <v>170</v>
-      </c>
-      <c r="C59" s="6" t="s">
-        <v>171</v>
-      </c>
-      <c r="D59" s="6" t="s">
-        <v>172</v>
       </c>
       <c r="E59">
         <v>40911</v>
@@ -2709,13 +2716,13 @@
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
+        <v>171</v>
+      </c>
+      <c r="B60" t="s">
+        <v>172</v>
+      </c>
+      <c r="C60" s="6" t="s">
         <v>173</v>
-      </c>
-      <c r="B60" t="s">
-        <v>174</v>
-      </c>
-      <c r="C60" s="6" t="s">
-        <v>175</v>
       </c>
       <c r="D60" s="1"/>
       <c r="E60">
@@ -2728,13 +2735,13 @@
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
+        <v>174</v>
+      </c>
+      <c r="B61" t="s">
+        <v>175</v>
+      </c>
+      <c r="C61" s="6" t="s">
         <v>176</v>
-      </c>
-      <c r="B61" t="s">
-        <v>177</v>
-      </c>
-      <c r="C61" s="6" t="s">
-        <v>178</v>
       </c>
       <c r="D61" s="1"/>
       <c r="E61">
@@ -2747,13 +2754,13 @@
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
+        <v>177</v>
+      </c>
+      <c r="B62" t="s">
+        <v>178</v>
+      </c>
+      <c r="C62" s="6" t="s">
         <v>179</v>
-      </c>
-      <c r="B62" t="s">
-        <v>180</v>
-      </c>
-      <c r="C62" s="6" t="s">
-        <v>181</v>
       </c>
       <c r="D62" s="1"/>
       <c r="E62">
@@ -2766,16 +2773,16 @@
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
+        <v>180</v>
+      </c>
+      <c r="B63" t="s">
+        <v>181</v>
+      </c>
+      <c r="C63" s="6" t="s">
         <v>182</v>
       </c>
-      <c r="B63" t="s">
+      <c r="D63" s="6" t="s">
         <v>183</v>
-      </c>
-      <c r="C63" s="6" t="s">
-        <v>184</v>
-      </c>
-      <c r="D63" s="6" t="s">
-        <v>185</v>
       </c>
       <c r="E63">
         <v>38638</v>
@@ -2787,13 +2794,13 @@
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
+        <v>184</v>
+      </c>
+      <c r="B64" t="s">
+        <v>185</v>
+      </c>
+      <c r="C64" s="6" t="s">
         <v>186</v>
-      </c>
-      <c r="B64" t="s">
-        <v>187</v>
-      </c>
-      <c r="C64" s="6" t="s">
-        <v>188</v>
       </c>
       <c r="D64" s="1"/>
       <c r="E64">
@@ -2806,16 +2813,16 @@
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
+        <v>187</v>
+      </c>
+      <c r="B65" t="s">
+        <v>188</v>
+      </c>
+      <c r="C65" s="6" t="s">
         <v>189</v>
       </c>
-      <c r="B65" t="s">
+      <c r="D65" s="6" t="s">
         <v>190</v>
-      </c>
-      <c r="C65" s="6" t="s">
-        <v>191</v>
-      </c>
-      <c r="D65" s="6" t="s">
-        <v>192</v>
       </c>
       <c r="E65">
         <v>38197</v>
@@ -2826,13 +2833,13 @@
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
+        <v>191</v>
+      </c>
+      <c r="B66" s="5" t="s">
+        <v>192</v>
+      </c>
+      <c r="C66" s="6" t="s">
         <v>193</v>
-      </c>
-      <c r="B66" s="5" t="s">
-        <v>194</v>
-      </c>
-      <c r="C66" s="6" t="s">
-        <v>195</v>
       </c>
       <c r="D66" s="1"/>
       <c r="E66">
@@ -2845,13 +2852,13 @@
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
+        <v>194</v>
+      </c>
+      <c r="B67" t="s">
+        <v>195</v>
+      </c>
+      <c r="C67" s="6" t="s">
         <v>196</v>
-      </c>
-      <c r="B67" t="s">
-        <v>197</v>
-      </c>
-      <c r="C67" s="6" t="s">
-        <v>198</v>
       </c>
       <c r="D67" s="1"/>
       <c r="E67">
@@ -2864,13 +2871,13 @@
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="B68" t="s">
         <v>55</v>
       </c>
       <c r="C68" s="6" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="D68" s="1"/>
       <c r="E68">
@@ -2883,13 +2890,13 @@
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="B69" t="s">
         <v>113</v>
       </c>
       <c r="C69" s="6" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="E69">
         <v>36139</v>
@@ -2900,13 +2907,13 @@
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="B70" t="s">
         <v>61</v>
       </c>
       <c r="C70" s="6" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="D70" s="1"/>
       <c r="E70">
@@ -2919,13 +2926,13 @@
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="B71" t="s">
         <v>30</v>
       </c>
       <c r="C71" s="6" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="D71" s="1"/>
       <c r="E71">
@@ -2938,13 +2945,13 @@
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="B72" t="s">
         <v>61</v>
       </c>
       <c r="C72" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="D72" s="1"/>
       <c r="E72">
@@ -2954,20 +2961,20 @@
         <v>11</v>
       </c>
       <c r="G72" s="10" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="H72" s="1"/>
       <c r="I72" s="1"/>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
+        <v>207</v>
+      </c>
+      <c r="B73" t="s">
+        <v>208</v>
+      </c>
+      <c r="C73" s="6" t="s">
         <v>209</v>
-      </c>
-      <c r="B73" t="s">
-        <v>210</v>
-      </c>
-      <c r="C73" s="6" t="s">
-        <v>211</v>
       </c>
       <c r="D73" s="1"/>
       <c r="E73">
@@ -2980,13 +2987,13 @@
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="B74" t="s">
         <v>55</v>
       </c>
       <c r="C74" s="6" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="D74" s="1"/>
       <c r="E74">
@@ -2999,16 +3006,16 @@
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="B75" t="s">
         <v>30</v>
       </c>
       <c r="C75" s="6" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="D75" s="6" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="E75">
         <v>29827</v>
@@ -3019,13 +3026,13 @@
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="B76" t="s">
         <v>61</v>
       </c>
       <c r="C76" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="D76" s="1"/>
       <c r="E76">
@@ -3035,23 +3042,23 @@
         <v>11</v>
       </c>
       <c r="G76" s="10" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="H76" s="9"/>
       <c r="I76" s="1"/>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
+        <v>217</v>
+      </c>
+      <c r="B77" t="s">
+        <v>218</v>
+      </c>
+      <c r="C77" s="6" t="s">
         <v>219</v>
       </c>
-      <c r="B77" t="s">
+      <c r="D77" s="6" t="s">
         <v>220</v>
-      </c>
-      <c r="C77" s="6" t="s">
-        <v>221</v>
-      </c>
-      <c r="D77" s="6" t="s">
-        <v>222</v>
       </c>
       <c r="E77">
         <v>29516</v>
@@ -3063,10 +3070,10 @@
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="B78" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="D78" s="1"/>
       <c r="E78">
@@ -3079,16 +3086,16 @@
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="B79" t="s">
         <v>33</v>
       </c>
       <c r="C79" s="6" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="D79" s="6" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="E79">
         <v>27743</v>
@@ -3100,13 +3107,13 @@
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
+        <v>226</v>
+      </c>
+      <c r="B80" t="s">
+        <v>227</v>
+      </c>
+      <c r="C80" s="6" t="s">
         <v>228</v>
-      </c>
-      <c r="B80" t="s">
-        <v>229</v>
-      </c>
-      <c r="C80" s="6" t="s">
-        <v>230</v>
       </c>
       <c r="D80" s="1"/>
       <c r="E80">
@@ -3119,13 +3126,13 @@
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="B81" t="s">
         <v>19</v>
       </c>
       <c r="C81" s="6" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="D81" s="1"/>
       <c r="E81">
@@ -3138,13 +3145,13 @@
     </row>
     <row r="82" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
+        <v>231</v>
+      </c>
+      <c r="B82" s="3" t="s">
+        <v>232</v>
+      </c>
+      <c r="C82" s="6" t="s">
         <v>233</v>
-      </c>
-      <c r="B82" s="3" t="s">
-        <v>234</v>
-      </c>
-      <c r="C82" s="6" t="s">
-        <v>235</v>
       </c>
       <c r="D82" s="1"/>
       <c r="E82">
@@ -3157,13 +3164,13 @@
     </row>
     <row r="83" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
+        <v>234</v>
+      </c>
+      <c r="B83" t="s">
+        <v>235</v>
+      </c>
+      <c r="C83" s="6" t="s">
         <v>236</v>
-      </c>
-      <c r="B83" t="s">
-        <v>237</v>
-      </c>
-      <c r="C83" s="6" t="s">
-        <v>238</v>
       </c>
       <c r="E83">
         <v>25028</v>
@@ -3174,13 +3181,13 @@
     </row>
     <row r="84" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
+        <v>237</v>
+      </c>
+      <c r="B84" t="s">
+        <v>238</v>
+      </c>
+      <c r="C84" s="6" t="s">
         <v>239</v>
-      </c>
-      <c r="B84" t="s">
-        <v>240</v>
-      </c>
-      <c r="C84" s="6" t="s">
-        <v>241</v>
       </c>
       <c r="D84" s="1"/>
       <c r="E84">
@@ -3193,16 +3200,16 @@
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
+        <v>240</v>
+      </c>
+      <c r="B85" t="s">
+        <v>241</v>
+      </c>
+      <c r="C85" s="6" t="s">
         <v>242</v>
       </c>
-      <c r="B85" t="s">
+      <c r="D85" s="6" t="s">
         <v>243</v>
-      </c>
-      <c r="C85" s="6" t="s">
-        <v>244</v>
-      </c>
-      <c r="D85" s="6" t="s">
-        <v>245</v>
       </c>
       <c r="E85">
         <v>22988</v>
@@ -3213,13 +3220,13 @@
     </row>
     <row r="86" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
+        <v>244</v>
+      </c>
+      <c r="B86" t="s">
+        <v>245</v>
+      </c>
+      <c r="C86" s="6" t="s">
         <v>246</v>
-      </c>
-      <c r="B86" t="s">
-        <v>247</v>
-      </c>
-      <c r="C86" s="6" t="s">
-        <v>248</v>
       </c>
       <c r="D86" s="1"/>
       <c r="E86">
@@ -3232,13 +3239,13 @@
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="B87" t="s">
         <v>71</v>
       </c>
       <c r="C87" s="6" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="D87" s="1"/>
       <c r="E87">
@@ -3251,13 +3258,13 @@
     </row>
     <row r="88" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
+        <v>249</v>
+      </c>
+      <c r="B88" t="s">
+        <v>250</v>
+      </c>
+      <c r="C88" s="6" t="s">
         <v>251</v>
-      </c>
-      <c r="B88" t="s">
-        <v>252</v>
-      </c>
-      <c r="C88" s="6" t="s">
-        <v>253</v>
       </c>
       <c r="D88" s="1"/>
       <c r="E88">
@@ -3270,13 +3277,13 @@
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="B89" t="s">
         <v>55</v>
       </c>
       <c r="C89" s="6" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="D89" s="1"/>
       <c r="E89">
@@ -3289,13 +3296,13 @@
     </row>
     <row r="90" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
+        <v>254</v>
+      </c>
+      <c r="B90" t="s">
+        <v>255</v>
+      </c>
+      <c r="C90" s="6" t="s">
         <v>256</v>
-      </c>
-      <c r="B90" t="s">
-        <v>257</v>
-      </c>
-      <c r="C90" s="6" t="s">
-        <v>258</v>
       </c>
       <c r="D90" s="1"/>
       <c r="E90">
@@ -3308,13 +3315,13 @@
     </row>
     <row r="91" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="B91" t="s">
         <v>61</v>
       </c>
       <c r="C91" s="6" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="E91">
         <v>20514</v>
@@ -3325,13 +3332,13 @@
     </row>
     <row r="92" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
+        <v>259</v>
+      </c>
+      <c r="B92" t="s">
+        <v>260</v>
+      </c>
+      <c r="C92" s="6" t="s">
         <v>261</v>
-      </c>
-      <c r="B92" t="s">
-        <v>262</v>
-      </c>
-      <c r="C92" s="6" t="s">
-        <v>263</v>
       </c>
       <c r="E92">
         <v>20133</v>
@@ -3342,13 +3349,13 @@
     </row>
     <row r="93" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
+        <v>262</v>
+      </c>
+      <c r="B93" t="s">
+        <v>263</v>
+      </c>
+      <c r="C93" s="6" t="s">
         <v>264</v>
-      </c>
-      <c r="B93" t="s">
-        <v>265</v>
-      </c>
-      <c r="C93" s="6" t="s">
-        <v>266</v>
       </c>
       <c r="D93" s="1"/>
       <c r="E93">
@@ -3361,13 +3368,13 @@
     </row>
     <row r="94" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="B94" t="s">
         <v>91</v>
       </c>
       <c r="C94" s="6" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="E94">
         <v>14272</v>
@@ -3378,13 +3385,13 @@
     </row>
     <row r="95" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="B95" t="s">
         <v>55</v>
       </c>
       <c r="C95" s="6" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="D95" s="1"/>
       <c r="E95">
@@ -3397,13 +3404,13 @@
     </row>
     <row r="96" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="B96" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="C96" s="6" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="E96">
         <v>6178</v>
@@ -3414,13 +3421,13 @@
     </row>
     <row r="97" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="B97" t="s">
         <v>61</v>
       </c>
       <c r="C97" s="6" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="D97" s="1"/>
       <c r="E97">
@@ -3430,20 +3437,20 @@
         <v>11</v>
       </c>
       <c r="G97" s="10" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="H97" s="8"/>
       <c r="I97" s="1"/>
     </row>
     <row r="98" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="B98" t="s">
         <v>61</v>
       </c>
       <c r="C98" s="6" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="E98">
         <v>3401</v>
@@ -3452,18 +3459,18 @@
         <v>11</v>
       </c>
       <c r="G98" s="12" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
     </row>
     <row r="99" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
+        <v>275</v>
+      </c>
+      <c r="B99" t="s">
+        <v>276</v>
+      </c>
+      <c r="C99" s="6" t="s">
         <v>277</v>
-      </c>
-      <c r="B99" t="s">
-        <v>278</v>
-      </c>
-      <c r="C99" s="6" t="s">
-        <v>279</v>
       </c>
       <c r="E99">
         <v>1807</v>

</xml_diff>